<commit_message>
nuevo modelo de base de datos relacional
</commit_message>
<xml_diff>
--- a/uploads/backup.xlsx
+++ b/uploads/backup.xlsx
@@ -493,6 +493,9 @@
       <c r="J2" t="n">
         <v>1</v>
       </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>Básica Rama</t>
@@ -562,6 +565,9 @@
       <c r="J3" t="n">
         <v>1</v>
       </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>Básica Rama</t>
@@ -631,6 +637,9 @@
       <c r="J4" t="n">
         <v>1</v>
       </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>Básica Rama</t>
@@ -700,6 +709,9 @@
       <c r="J5" t="n">
         <v>1</v>
       </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>Básica Rama</t>
@@ -769,6 +781,9 @@
       <c r="J6" t="n">
         <v>1</v>
       </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -838,6 +853,9 @@
       <c r="J7" t="n">
         <v>1</v>
       </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -907,6 +925,9 @@
       <c r="J8" t="n">
         <v>1</v>
       </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -976,6 +997,9 @@
       <c r="J9" t="n">
         <v>1</v>
       </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1045,6 +1069,9 @@
       <c r="J10" t="n">
         <v>1</v>
       </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
       <c r="L10" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1114,6 +1141,9 @@
       <c r="J11" t="n">
         <v>1</v>
       </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
       <c r="L11" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1183,6 +1213,9 @@
       <c r="J12" t="n">
         <v>1</v>
       </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
       <c r="L12" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1252,6 +1285,9 @@
       <c r="J13" t="n">
         <v>1</v>
       </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1321,6 +1357,9 @@
       <c r="J14" t="n">
         <v>1</v>
       </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1390,6 +1429,9 @@
       <c r="J15" t="n">
         <v>1</v>
       </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1459,6 +1501,9 @@
       <c r="J16" t="n">
         <v>1</v>
       </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1528,6 +1573,9 @@
       <c r="J17" t="n">
         <v>1</v>
       </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1597,6 +1645,9 @@
       <c r="J18" t="n">
         <v>1</v>
       </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1666,6 +1717,9 @@
       <c r="J19" t="n">
         <v>1</v>
       </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1735,6 +1789,9 @@
       <c r="J20" t="n">
         <v>1</v>
       </c>
+      <c r="K20" t="n">
+        <v>1</v>
+      </c>
       <c r="L20" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1804,6 +1861,9 @@
       <c r="J21" t="n">
         <v>1</v>
       </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
       <c r="L21" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1873,6 +1933,9 @@
       <c r="J22" t="n">
         <v>1</v>
       </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -1942,6 +2005,9 @@
       <c r="J23" t="n">
         <v>1</v>
       </c>
+      <c r="K23" t="n">
+        <v>1</v>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2011,6 +2077,9 @@
       <c r="J24" t="n">
         <v>1</v>
       </c>
+      <c r="K24" t="n">
+        <v>1</v>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2080,6 +2149,9 @@
       <c r="J25" t="n">
         <v>1</v>
       </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
       <c r="L25" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2149,6 +2221,9 @@
       <c r="J26" t="n">
         <v>1</v>
       </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
       <c r="L26" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2218,6 +2293,9 @@
       <c r="J27" t="n">
         <v>1</v>
       </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
       <c r="L27" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2287,6 +2365,9 @@
       <c r="J28" t="n">
         <v>1</v>
       </c>
+      <c r="K28" t="n">
+        <v>1</v>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2356,6 +2437,9 @@
       <c r="J29" t="n">
         <v>1</v>
       </c>
+      <c r="K29" t="n">
+        <v>1</v>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2425,6 +2509,9 @@
       <c r="J30" t="n">
         <v>1</v>
       </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
       <c r="L30" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2494,6 +2581,9 @@
       <c r="J31" t="n">
         <v>1</v>
       </c>
+      <c r="K31" t="n">
+        <v>1</v>
+      </c>
       <c r="L31" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2563,6 +2653,9 @@
       <c r="J32" t="n">
         <v>1</v>
       </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
       <c r="L32" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2632,6 +2725,9 @@
       <c r="J33" t="n">
         <v>1</v>
       </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
       <c r="L33" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2701,6 +2797,9 @@
       <c r="J34" t="n">
         <v>1</v>
       </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
       <c r="L34" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2770,6 +2869,9 @@
       <c r="J35" t="n">
         <v>1</v>
       </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
       <c r="L35" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2839,6 +2941,9 @@
       <c r="J36" t="n">
         <v>1</v>
       </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
       <c r="L36" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2908,6 +3013,9 @@
       <c r="J37" t="n">
         <v>1</v>
       </c>
+      <c r="K37" t="n">
+        <v>1</v>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -2977,6 +3085,9 @@
       <c r="J38" t="n">
         <v>1</v>
       </c>
+      <c r="K38" t="n">
+        <v>1</v>
+      </c>
       <c r="L38" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3046,6 +3157,9 @@
       <c r="J39" t="n">
         <v>1</v>
       </c>
+      <c r="K39" t="n">
+        <v>1</v>
+      </c>
       <c r="L39" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3115,6 +3229,9 @@
       <c r="J40" t="n">
         <v>1</v>
       </c>
+      <c r="K40" t="n">
+        <v>1</v>
+      </c>
       <c r="L40" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3184,6 +3301,9 @@
       <c r="J41" t="n">
         <v>1</v>
       </c>
+      <c r="K41" t="n">
+        <v>1</v>
+      </c>
       <c r="L41" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3253,6 +3373,9 @@
       <c r="J42" t="n">
         <v>1</v>
       </c>
+      <c r="K42" t="n">
+        <v>1</v>
+      </c>
       <c r="L42" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3322,6 +3445,9 @@
       <c r="J43" t="n">
         <v>1</v>
       </c>
+      <c r="K43" t="n">
+        <v>1</v>
+      </c>
       <c r="L43" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3391,6 +3517,9 @@
       <c r="J44" t="n">
         <v>1</v>
       </c>
+      <c r="K44" t="n">
+        <v>1</v>
+      </c>
       <c r="L44" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3460,6 +3589,9 @@
       <c r="J45" t="n">
         <v>1</v>
       </c>
+      <c r="K45" t="n">
+        <v>1</v>
+      </c>
       <c r="L45" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3529,6 +3661,9 @@
       <c r="J46" t="n">
         <v>1</v>
       </c>
+      <c r="K46" t="n">
+        <v>1</v>
+      </c>
       <c r="L46" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3598,6 +3733,9 @@
       <c r="J47" t="n">
         <v>1</v>
       </c>
+      <c r="K47" t="n">
+        <v>1</v>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3667,6 +3805,9 @@
       <c r="J48" t="n">
         <v>1</v>
       </c>
+      <c r="K48" t="n">
+        <v>1</v>
+      </c>
       <c r="L48" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3736,6 +3877,9 @@
       <c r="J49" t="n">
         <v>1</v>
       </c>
+      <c r="K49" t="n">
+        <v>1</v>
+      </c>
       <c r="L49" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3805,6 +3949,9 @@
       <c r="J50" t="n">
         <v>1</v>
       </c>
+      <c r="K50" t="n">
+        <v>1</v>
+      </c>
       <c r="L50" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3874,6 +4021,9 @@
       <c r="J51" t="n">
         <v>1</v>
       </c>
+      <c r="K51" t="n">
+        <v>1</v>
+      </c>
       <c r="L51" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -3943,6 +4093,9 @@
       <c r="J52" t="n">
         <v>1</v>
       </c>
+      <c r="K52" t="n">
+        <v>1</v>
+      </c>
       <c r="L52" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -4012,6 +4165,9 @@
       <c r="J53" t="n">
         <v>1</v>
       </c>
+      <c r="K53" t="n">
+        <v>1</v>
+      </c>
       <c r="L53" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -4079,6 +4235,9 @@
         </is>
       </c>
       <c r="J54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K54" t="n">
         <v>2</v>
       </c>
       <c r="L54" t="inlineStr">
@@ -4148,6 +4307,9 @@
         </is>
       </c>
       <c r="J55" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" t="n">
         <v>2</v>
       </c>
       <c r="L55" t="inlineStr">
@@ -4217,6 +4379,9 @@
         </is>
       </c>
       <c r="J56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" t="n">
         <v>2</v>
       </c>
       <c r="L56" t="inlineStr">
@@ -4286,6 +4451,9 @@
         </is>
       </c>
       <c r="J57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" t="n">
         <v>2</v>
       </c>
       <c r="L57" t="inlineStr">
@@ -4355,6 +4523,9 @@
         </is>
       </c>
       <c r="J58" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" t="n">
         <v>2</v>
       </c>
       <c r="L58" t="inlineStr">
@@ -4424,6 +4595,9 @@
         </is>
       </c>
       <c r="J59" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" t="n">
         <v>2</v>
       </c>
       <c r="L59" t="inlineStr">
@@ -4493,6 +4667,9 @@
         </is>
       </c>
       <c r="J60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" t="n">
         <v>2</v>
       </c>
       <c r="L60" t="inlineStr">
@@ -4562,6 +4739,9 @@
         </is>
       </c>
       <c r="J61" t="n">
+        <v>1</v>
+      </c>
+      <c r="K61" t="n">
         <v>2</v>
       </c>
       <c r="L61" t="inlineStr">
@@ -4631,6 +4811,9 @@
         </is>
       </c>
       <c r="J62" t="n">
+        <v>1</v>
+      </c>
+      <c r="K62" t="n">
         <v>2</v>
       </c>
       <c r="L62" t="inlineStr">
@@ -4700,6 +4883,9 @@
         </is>
       </c>
       <c r="J63" t="n">
+        <v>1</v>
+      </c>
+      <c r="K63" t="n">
         <v>2</v>
       </c>
       <c r="L63" t="inlineStr">
@@ -4769,6 +4955,9 @@
         </is>
       </c>
       <c r="J64" t="n">
+        <v>1</v>
+      </c>
+      <c r="K64" t="n">
         <v>2</v>
       </c>
       <c r="L64" t="inlineStr">
@@ -4838,6 +5027,9 @@
         </is>
       </c>
       <c r="J65" t="n">
+        <v>1</v>
+      </c>
+      <c r="K65" t="n">
         <v>2</v>
       </c>
       <c r="L65" t="inlineStr">
@@ -4907,6 +5099,9 @@
         </is>
       </c>
       <c r="J66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K66" t="n">
         <v>2</v>
       </c>
       <c r="L66" t="inlineStr">
@@ -4976,6 +5171,9 @@
         </is>
       </c>
       <c r="J67" t="n">
+        <v>1</v>
+      </c>
+      <c r="K67" t="n">
         <v>2</v>
       </c>
       <c r="L67" t="inlineStr">
@@ -5045,6 +5243,9 @@
         </is>
       </c>
       <c r="J68" t="n">
+        <v>1</v>
+      </c>
+      <c r="K68" t="n">
         <v>2</v>
       </c>
       <c r="L68" t="inlineStr">
@@ -5114,6 +5315,9 @@
         </is>
       </c>
       <c r="J69" t="n">
+        <v>1</v>
+      </c>
+      <c r="K69" t="n">
         <v>2</v>
       </c>
       <c r="L69" t="inlineStr">
@@ -5183,6 +5387,9 @@
         </is>
       </c>
       <c r="J70" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" t="n">
         <v>2</v>
       </c>
       <c r="L70" t="inlineStr">
@@ -5252,6 +5459,9 @@
         </is>
       </c>
       <c r="J71" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" t="n">
         <v>2</v>
       </c>
       <c r="L71" t="inlineStr">
@@ -5321,6 +5531,9 @@
         </is>
       </c>
       <c r="J72" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" t="n">
         <v>2</v>
       </c>
       <c r="L72" t="inlineStr">
@@ -5390,6 +5603,9 @@
         </is>
       </c>
       <c r="J73" t="n">
+        <v>1</v>
+      </c>
+      <c r="K73" t="n">
         <v>2</v>
       </c>
       <c r="L73" t="inlineStr">
@@ -5459,6 +5675,9 @@
         </is>
       </c>
       <c r="J74" t="n">
+        <v>1</v>
+      </c>
+      <c r="K74" t="n">
         <v>2</v>
       </c>
       <c r="L74" t="inlineStr">
@@ -5528,6 +5747,9 @@
         </is>
       </c>
       <c r="J75" t="n">
+        <v>1</v>
+      </c>
+      <c r="K75" t="n">
         <v>2</v>
       </c>
       <c r="L75" t="inlineStr">
@@ -5597,6 +5819,9 @@
         </is>
       </c>
       <c r="J76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K76" t="n">
         <v>2</v>
       </c>
       <c r="L76" t="inlineStr">
@@ -5666,6 +5891,9 @@
         </is>
       </c>
       <c r="J77" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" t="n">
         <v>2</v>
       </c>
       <c r="L77" t="inlineStr">
@@ -5735,6 +5963,9 @@
         </is>
       </c>
       <c r="J78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K78" t="n">
         <v>2</v>
       </c>
       <c r="L78" t="inlineStr">
@@ -5804,6 +6035,9 @@
         </is>
       </c>
       <c r="J79" t="n">
+        <v>1</v>
+      </c>
+      <c r="K79" t="n">
         <v>2</v>
       </c>
       <c r="L79" t="inlineStr">
@@ -5873,6 +6107,9 @@
         </is>
       </c>
       <c r="J80" t="n">
+        <v>1</v>
+      </c>
+      <c r="K80" t="n">
         <v>2</v>
       </c>
       <c r="L80" t="inlineStr">
@@ -5942,6 +6179,9 @@
         </is>
       </c>
       <c r="J81" t="n">
+        <v>1</v>
+      </c>
+      <c r="K81" t="n">
         <v>2</v>
       </c>
       <c r="L81" t="inlineStr">
@@ -6011,6 +6251,9 @@
         </is>
       </c>
       <c r="J82" t="n">
+        <v>1</v>
+      </c>
+      <c r="K82" t="n">
         <v>2</v>
       </c>
       <c r="L82" t="inlineStr">
@@ -6080,6 +6323,9 @@
         </is>
       </c>
       <c r="J83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K83" t="n">
         <v>2</v>
       </c>
       <c r="L83" t="inlineStr">
@@ -6149,6 +6395,9 @@
         </is>
       </c>
       <c r="J84" t="n">
+        <v>1</v>
+      </c>
+      <c r="K84" t="n">
         <v>2</v>
       </c>
       <c r="L84" t="inlineStr">
@@ -6218,6 +6467,9 @@
         </is>
       </c>
       <c r="J85" t="n">
+        <v>1</v>
+      </c>
+      <c r="K85" t="n">
         <v>2</v>
       </c>
       <c r="L85" t="inlineStr">
@@ -6287,6 +6539,9 @@
         </is>
       </c>
       <c r="J86" t="n">
+        <v>1</v>
+      </c>
+      <c r="K86" t="n">
         <v>2</v>
       </c>
       <c r="L86" t="inlineStr">
@@ -6356,6 +6611,9 @@
         </is>
       </c>
       <c r="J87" t="n">
+        <v>1</v>
+      </c>
+      <c r="K87" t="n">
         <v>2</v>
       </c>
       <c r="L87" t="inlineStr">
@@ -6425,6 +6683,9 @@
         </is>
       </c>
       <c r="J88" t="n">
+        <v>1</v>
+      </c>
+      <c r="K88" t="n">
         <v>2</v>
       </c>
       <c r="L88" t="inlineStr">
@@ -6494,6 +6755,9 @@
         </is>
       </c>
       <c r="J89" t="n">
+        <v>1</v>
+      </c>
+      <c r="K89" t="n">
         <v>2</v>
       </c>
       <c r="L89" t="inlineStr">
@@ -6563,6 +6827,9 @@
         </is>
       </c>
       <c r="J90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K90" t="n">
         <v>2</v>
       </c>
       <c r="L90" t="inlineStr">
@@ -6632,6 +6899,9 @@
         </is>
       </c>
       <c r="J91" t="n">
+        <v>1</v>
+      </c>
+      <c r="K91" t="n">
         <v>2</v>
       </c>
       <c r="L91" t="inlineStr">
@@ -6701,6 +6971,9 @@
         </is>
       </c>
       <c r="J92" t="n">
+        <v>1</v>
+      </c>
+      <c r="K92" t="n">
         <v>2</v>
       </c>
       <c r="L92" t="inlineStr">
@@ -6770,6 +7043,9 @@
         </is>
       </c>
       <c r="J93" t="n">
+        <v>2</v>
+      </c>
+      <c r="K93" t="n">
         <v>1</v>
       </c>
       <c r="L93" t="inlineStr">
@@ -6839,6 +7115,9 @@
         </is>
       </c>
       <c r="J94" t="n">
+        <v>2</v>
+      </c>
+      <c r="K94" t="n">
         <v>1</v>
       </c>
       <c r="L94" t="inlineStr">
@@ -6908,6 +7187,9 @@
         </is>
       </c>
       <c r="J95" t="n">
+        <v>2</v>
+      </c>
+      <c r="K95" t="n">
         <v>1</v>
       </c>
       <c r="L95" t="inlineStr">
@@ -6977,6 +7259,9 @@
         </is>
       </c>
       <c r="J96" t="n">
+        <v>2</v>
+      </c>
+      <c r="K96" t="n">
         <v>1</v>
       </c>
       <c r="L96" t="inlineStr">
@@ -7046,6 +7331,9 @@
         </is>
       </c>
       <c r="J97" t="n">
+        <v>2</v>
+      </c>
+      <c r="K97" t="n">
         <v>1</v>
       </c>
       <c r="L97" t="inlineStr">
@@ -7115,6 +7403,9 @@
         </is>
       </c>
       <c r="J98" t="n">
+        <v>2</v>
+      </c>
+      <c r="K98" t="n">
         <v>1</v>
       </c>
       <c r="L98" t="inlineStr">
@@ -7184,6 +7475,9 @@
         </is>
       </c>
       <c r="J99" t="n">
+        <v>2</v>
+      </c>
+      <c r="K99" t="n">
         <v>1</v>
       </c>
       <c r="L99" t="inlineStr">
@@ -7253,6 +7547,9 @@
         </is>
       </c>
       <c r="J100" t="n">
+        <v>2</v>
+      </c>
+      <c r="K100" t="n">
         <v>1</v>
       </c>
       <c r="L100" t="inlineStr">
@@ -7322,6 +7619,9 @@
         </is>
       </c>
       <c r="J101" t="n">
+        <v>2</v>
+      </c>
+      <c r="K101" t="n">
         <v>1</v>
       </c>
       <c r="L101" t="inlineStr">
@@ -7391,6 +7691,9 @@
         </is>
       </c>
       <c r="J102" t="n">
+        <v>2</v>
+      </c>
+      <c r="K102" t="n">
         <v>1</v>
       </c>
       <c r="L102" t="inlineStr">
@@ -7460,6 +7763,9 @@
         </is>
       </c>
       <c r="J103" t="n">
+        <v>2</v>
+      </c>
+      <c r="K103" t="n">
         <v>1</v>
       </c>
       <c r="L103" t="inlineStr">
@@ -7529,6 +7835,9 @@
         </is>
       </c>
       <c r="J104" t="n">
+        <v>2</v>
+      </c>
+      <c r="K104" t="n">
         <v>1</v>
       </c>
       <c r="L104" t="inlineStr">
@@ -7598,6 +7907,9 @@
         </is>
       </c>
       <c r="J105" t="n">
+        <v>2</v>
+      </c>
+      <c r="K105" t="n">
         <v>1</v>
       </c>
       <c r="L105" t="inlineStr">
@@ -7667,6 +7979,9 @@
         </is>
       </c>
       <c r="J106" t="n">
+        <v>2</v>
+      </c>
+      <c r="K106" t="n">
         <v>1</v>
       </c>
       <c r="L106" t="inlineStr">
@@ -7736,6 +8051,9 @@
         </is>
       </c>
       <c r="J107" t="n">
+        <v>2</v>
+      </c>
+      <c r="K107" t="n">
         <v>1</v>
       </c>
       <c r="L107" t="inlineStr">
@@ -7805,6 +8123,9 @@
         </is>
       </c>
       <c r="J108" t="n">
+        <v>2</v>
+      </c>
+      <c r="K108" t="n">
         <v>1</v>
       </c>
       <c r="L108" t="inlineStr">
@@ -7874,6 +8195,9 @@
         </is>
       </c>
       <c r="J109" t="n">
+        <v>2</v>
+      </c>
+      <c r="K109" t="n">
         <v>1</v>
       </c>
       <c r="L109" t="inlineStr">
@@ -7943,6 +8267,9 @@
         </is>
       </c>
       <c r="J110" t="n">
+        <v>2</v>
+      </c>
+      <c r="K110" t="n">
         <v>1</v>
       </c>
       <c r="L110" t="inlineStr">
@@ -8012,6 +8339,9 @@
         </is>
       </c>
       <c r="J111" t="n">
+        <v>2</v>
+      </c>
+      <c r="K111" t="n">
         <v>1</v>
       </c>
       <c r="L111" t="inlineStr">
@@ -8081,6 +8411,9 @@
         </is>
       </c>
       <c r="J112" t="n">
+        <v>2</v>
+      </c>
+      <c r="K112" t="n">
         <v>1</v>
       </c>
       <c r="L112" t="inlineStr">
@@ -8150,6 +8483,9 @@
         </is>
       </c>
       <c r="J113" t="n">
+        <v>2</v>
+      </c>
+      <c r="K113" t="n">
         <v>1</v>
       </c>
       <c r="L113" t="inlineStr">
@@ -8219,6 +8555,9 @@
         </is>
       </c>
       <c r="J114" t="n">
+        <v>2</v>
+      </c>
+      <c r="K114" t="n">
         <v>1</v>
       </c>
       <c r="L114" t="inlineStr">
@@ -8288,6 +8627,9 @@
         </is>
       </c>
       <c r="J115" t="n">
+        <v>2</v>
+      </c>
+      <c r="K115" t="n">
         <v>1</v>
       </c>
       <c r="L115" t="inlineStr">
@@ -8357,6 +8699,9 @@
         </is>
       </c>
       <c r="J116" t="n">
+        <v>2</v>
+      </c>
+      <c r="K116" t="n">
         <v>1</v>
       </c>
       <c r="L116" t="inlineStr">
@@ -8426,6 +8771,9 @@
         </is>
       </c>
       <c r="J117" t="n">
+        <v>2</v>
+      </c>
+      <c r="K117" t="n">
         <v>1</v>
       </c>
       <c r="L117" t="inlineStr">
@@ -8495,6 +8843,9 @@
         </is>
       </c>
       <c r="J118" t="n">
+        <v>2</v>
+      </c>
+      <c r="K118" t="n">
         <v>1</v>
       </c>
       <c r="L118" t="inlineStr">
@@ -8564,6 +8915,9 @@
         </is>
       </c>
       <c r="J119" t="n">
+        <v>2</v>
+      </c>
+      <c r="K119" t="n">
         <v>1</v>
       </c>
       <c r="L119" t="inlineStr">
@@ -8633,6 +8987,9 @@
         </is>
       </c>
       <c r="J120" t="n">
+        <v>2</v>
+      </c>
+      <c r="K120" t="n">
         <v>1</v>
       </c>
       <c r="L120" t="inlineStr">
@@ -8702,6 +9059,9 @@
         </is>
       </c>
       <c r="J121" t="n">
+        <v>2</v>
+      </c>
+      <c r="K121" t="n">
         <v>1</v>
       </c>
       <c r="L121" t="inlineStr">
@@ -8771,6 +9131,9 @@
         </is>
       </c>
       <c r="J122" t="n">
+        <v>2</v>
+      </c>
+      <c r="K122" t="n">
         <v>1</v>
       </c>
       <c r="L122" t="inlineStr">
@@ -8840,6 +9203,9 @@
         </is>
       </c>
       <c r="J123" t="n">
+        <v>2</v>
+      </c>
+      <c r="K123" t="n">
         <v>1</v>
       </c>
       <c r="L123" t="inlineStr">
@@ -8909,6 +9275,9 @@
         </is>
       </c>
       <c r="J124" t="n">
+        <v>2</v>
+      </c>
+      <c r="K124" t="n">
         <v>1</v>
       </c>
       <c r="L124" t="inlineStr">
@@ -8978,6 +9347,9 @@
         </is>
       </c>
       <c r="J125" t="n">
+        <v>2</v>
+      </c>
+      <c r="K125" t="n">
         <v>1</v>
       </c>
       <c r="L125" t="inlineStr">
@@ -9047,6 +9419,9 @@
         </is>
       </c>
       <c r="J126" t="n">
+        <v>2</v>
+      </c>
+      <c r="K126" t="n">
         <v>1</v>
       </c>
       <c r="L126" t="inlineStr">
@@ -9116,6 +9491,9 @@
         </is>
       </c>
       <c r="J127" t="n">
+        <v>2</v>
+      </c>
+      <c r="K127" t="n">
         <v>1</v>
       </c>
       <c r="L127" t="inlineStr">
@@ -9185,6 +9563,9 @@
         </is>
       </c>
       <c r="J128" t="n">
+        <v>2</v>
+      </c>
+      <c r="K128" t="n">
         <v>1</v>
       </c>
       <c r="L128" t="inlineStr">
@@ -9254,6 +9635,9 @@
         </is>
       </c>
       <c r="J129" t="n">
+        <v>2</v>
+      </c>
+      <c r="K129" t="n">
         <v>1</v>
       </c>
       <c r="L129" t="inlineStr">
@@ -9323,6 +9707,9 @@
         </is>
       </c>
       <c r="J130" t="n">
+        <v>2</v>
+      </c>
+      <c r="K130" t="n">
         <v>1</v>
       </c>
       <c r="L130" t="inlineStr">
@@ -9392,6 +9779,9 @@
         </is>
       </c>
       <c r="J131" t="n">
+        <v>2</v>
+      </c>
+      <c r="K131" t="n">
         <v>1</v>
       </c>
       <c r="L131" t="inlineStr">
@@ -9461,6 +9851,9 @@
         </is>
       </c>
       <c r="J132" t="n">
+        <v>2</v>
+      </c>
+      <c r="K132" t="n">
         <v>1</v>
       </c>
       <c r="L132" t="inlineStr">
@@ -9532,6 +9925,9 @@
       <c r="J133" t="n">
         <v>2</v>
       </c>
+      <c r="K133" t="n">
+        <v>2</v>
+      </c>
       <c r="L133" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -9601,6 +9997,9 @@
       <c r="J134" t="n">
         <v>2</v>
       </c>
+      <c r="K134" t="n">
+        <v>2</v>
+      </c>
       <c r="L134" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -9670,6 +10069,9 @@
       <c r="J135" t="n">
         <v>2</v>
       </c>
+      <c r="K135" t="n">
+        <v>2</v>
+      </c>
       <c r="L135" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -9739,6 +10141,9 @@
       <c r="J136" t="n">
         <v>2</v>
       </c>
+      <c r="K136" t="n">
+        <v>2</v>
+      </c>
       <c r="L136" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -9808,6 +10213,9 @@
       <c r="J137" t="n">
         <v>2</v>
       </c>
+      <c r="K137" t="n">
+        <v>2</v>
+      </c>
       <c r="L137" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -9877,6 +10285,9 @@
       <c r="J138" t="n">
         <v>2</v>
       </c>
+      <c r="K138" t="n">
+        <v>2</v>
+      </c>
       <c r="L138" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -9946,6 +10357,9 @@
       <c r="J139" t="n">
         <v>2</v>
       </c>
+      <c r="K139" t="n">
+        <v>2</v>
+      </c>
       <c r="L139" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10015,6 +10429,9 @@
       <c r="J140" t="n">
         <v>2</v>
       </c>
+      <c r="K140" t="n">
+        <v>2</v>
+      </c>
       <c r="L140" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10084,6 +10501,9 @@
       <c r="J141" t="n">
         <v>2</v>
       </c>
+      <c r="K141" t="n">
+        <v>2</v>
+      </c>
       <c r="L141" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10153,6 +10573,9 @@
       <c r="J142" t="n">
         <v>2</v>
       </c>
+      <c r="K142" t="n">
+        <v>2</v>
+      </c>
       <c r="L142" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10222,6 +10645,9 @@
       <c r="J143" t="n">
         <v>2</v>
       </c>
+      <c r="K143" t="n">
+        <v>2</v>
+      </c>
       <c r="L143" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10291,6 +10717,9 @@
       <c r="J144" t="n">
         <v>2</v>
       </c>
+      <c r="K144" t="n">
+        <v>2</v>
+      </c>
       <c r="L144" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10360,6 +10789,9 @@
       <c r="J145" t="n">
         <v>2</v>
       </c>
+      <c r="K145" t="n">
+        <v>2</v>
+      </c>
       <c r="L145" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10429,6 +10861,9 @@
       <c r="J146" t="n">
         <v>2</v>
       </c>
+      <c r="K146" t="n">
+        <v>2</v>
+      </c>
       <c r="L146" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10498,6 +10933,9 @@
       <c r="J147" t="n">
         <v>2</v>
       </c>
+      <c r="K147" t="n">
+        <v>2</v>
+      </c>
       <c r="L147" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10567,6 +11005,9 @@
       <c r="J148" t="n">
         <v>2</v>
       </c>
+      <c r="K148" t="n">
+        <v>2</v>
+      </c>
       <c r="L148" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10636,6 +11077,9 @@
       <c r="J149" t="n">
         <v>2</v>
       </c>
+      <c r="K149" t="n">
+        <v>2</v>
+      </c>
       <c r="L149" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10705,6 +11149,9 @@
       <c r="J150" t="n">
         <v>2</v>
       </c>
+      <c r="K150" t="n">
+        <v>2</v>
+      </c>
       <c r="L150" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10774,6 +11221,9 @@
       <c r="J151" t="n">
         <v>2</v>
       </c>
+      <c r="K151" t="n">
+        <v>2</v>
+      </c>
       <c r="L151" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10843,6 +11293,9 @@
       <c r="J152" t="n">
         <v>2</v>
       </c>
+      <c r="K152" t="n">
+        <v>2</v>
+      </c>
       <c r="L152" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10912,6 +11365,9 @@
       <c r="J153" t="n">
         <v>2</v>
       </c>
+      <c r="K153" t="n">
+        <v>2</v>
+      </c>
       <c r="L153" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -10981,6 +11437,9 @@
       <c r="J154" t="n">
         <v>2</v>
       </c>
+      <c r="K154" t="n">
+        <v>2</v>
+      </c>
       <c r="L154" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11050,6 +11509,9 @@
       <c r="J155" t="n">
         <v>2</v>
       </c>
+      <c r="K155" t="n">
+        <v>2</v>
+      </c>
       <c r="L155" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11119,6 +11581,9 @@
       <c r="J156" t="n">
         <v>2</v>
       </c>
+      <c r="K156" t="n">
+        <v>2</v>
+      </c>
       <c r="L156" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11188,6 +11653,9 @@
       <c r="J157" t="n">
         <v>2</v>
       </c>
+      <c r="K157" t="n">
+        <v>2</v>
+      </c>
       <c r="L157" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11257,6 +11725,9 @@
       <c r="J158" t="n">
         <v>2</v>
       </c>
+      <c r="K158" t="n">
+        <v>2</v>
+      </c>
       <c r="L158" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11326,6 +11797,9 @@
       <c r="J159" t="n">
         <v>2</v>
       </c>
+      <c r="K159" t="n">
+        <v>2</v>
+      </c>
       <c r="L159" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11395,6 +11869,9 @@
       <c r="J160" t="n">
         <v>2</v>
       </c>
+      <c r="K160" t="n">
+        <v>2</v>
+      </c>
       <c r="L160" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11464,6 +11941,9 @@
       <c r="J161" t="n">
         <v>2</v>
       </c>
+      <c r="K161" t="n">
+        <v>2</v>
+      </c>
       <c r="L161" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11533,6 +12013,9 @@
       <c r="J162" t="n">
         <v>2</v>
       </c>
+      <c r="K162" t="n">
+        <v>2</v>
+      </c>
       <c r="L162" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11602,6 +12085,9 @@
       <c r="J163" t="n">
         <v>2</v>
       </c>
+      <c r="K163" t="n">
+        <v>2</v>
+      </c>
       <c r="L163" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11671,6 +12157,9 @@
       <c r="J164" t="n">
         <v>2</v>
       </c>
+      <c r="K164" t="n">
+        <v>2</v>
+      </c>
       <c r="L164" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11740,6 +12229,9 @@
       <c r="J165" t="n">
         <v>2</v>
       </c>
+      <c r="K165" t="n">
+        <v>2</v>
+      </c>
       <c r="L165" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11809,6 +12301,9 @@
       <c r="J166" t="n">
         <v>2</v>
       </c>
+      <c r="K166" t="n">
+        <v>2</v>
+      </c>
       <c r="L166" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11878,6 +12373,9 @@
       <c r="J167" t="n">
         <v>2</v>
       </c>
+      <c r="K167" t="n">
+        <v>2</v>
+      </c>
       <c r="L167" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -11947,6 +12445,9 @@
       <c r="J168" t="n">
         <v>2</v>
       </c>
+      <c r="K168" t="n">
+        <v>2</v>
+      </c>
       <c r="L168" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12016,6 +12517,9 @@
       <c r="J169" t="n">
         <v>2</v>
       </c>
+      <c r="K169" t="n">
+        <v>2</v>
+      </c>
       <c r="L169" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12085,6 +12589,9 @@
       <c r="J170" t="n">
         <v>2</v>
       </c>
+      <c r="K170" t="n">
+        <v>2</v>
+      </c>
       <c r="L170" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12154,6 +12661,9 @@
       <c r="J171" t="n">
         <v>2</v>
       </c>
+      <c r="K171" t="n">
+        <v>2</v>
+      </c>
       <c r="L171" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12223,6 +12733,9 @@
       <c r="J172" t="n">
         <v>2</v>
       </c>
+      <c r="K172" t="n">
+        <v>2</v>
+      </c>
       <c r="L172" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12292,6 +12805,9 @@
       <c r="J173" t="n">
         <v>2</v>
       </c>
+      <c r="K173" t="n">
+        <v>2</v>
+      </c>
       <c r="L173" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12361,6 +12877,9 @@
       <c r="J174" t="n">
         <v>2</v>
       </c>
+      <c r="K174" t="n">
+        <v>2</v>
+      </c>
       <c r="L174" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12430,6 +12949,9 @@
       <c r="J175" t="n">
         <v>2</v>
       </c>
+      <c r="K175" t="n">
+        <v>2</v>
+      </c>
       <c r="L175" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12499,6 +13021,9 @@
       <c r="J176" t="n">
         <v>2</v>
       </c>
+      <c r="K176" t="n">
+        <v>2</v>
+      </c>
       <c r="L176" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12568,6 +13093,9 @@
       <c r="J177" t="n">
         <v>2</v>
       </c>
+      <c r="K177" t="n">
+        <v>2</v>
+      </c>
       <c r="L177" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12637,6 +13165,9 @@
       <c r="J178" t="n">
         <v>2</v>
       </c>
+      <c r="K178" t="n">
+        <v>2</v>
+      </c>
       <c r="L178" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12706,6 +13237,9 @@
       <c r="J179" t="n">
         <v>2</v>
       </c>
+      <c r="K179" t="n">
+        <v>2</v>
+      </c>
       <c r="L179" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12775,6 +13309,9 @@
       <c r="J180" t="n">
         <v>2</v>
       </c>
+      <c r="K180" t="n">
+        <v>2</v>
+      </c>
       <c r="L180" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12844,6 +13381,9 @@
       <c r="J181" t="n">
         <v>2</v>
       </c>
+      <c r="K181" t="n">
+        <v>2</v>
+      </c>
       <c r="L181" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12913,6 +13453,9 @@
       <c r="J182" t="n">
         <v>2</v>
       </c>
+      <c r="K182" t="n">
+        <v>2</v>
+      </c>
       <c r="L182" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -12980,6 +13523,9 @@
         </is>
       </c>
       <c r="J183" t="n">
+        <v>3</v>
+      </c>
+      <c r="K183" t="n">
         <v>1</v>
       </c>
       <c r="L183" t="inlineStr">
@@ -13049,6 +13595,9 @@
         </is>
       </c>
       <c r="J184" t="n">
+        <v>3</v>
+      </c>
+      <c r="K184" t="n">
         <v>1</v>
       </c>
       <c r="L184" t="inlineStr">
@@ -13118,6 +13667,9 @@
         </is>
       </c>
       <c r="J185" t="n">
+        <v>3</v>
+      </c>
+      <c r="K185" t="n">
         <v>1</v>
       </c>
       <c r="L185" t="inlineStr">
@@ -13187,6 +13739,9 @@
         </is>
       </c>
       <c r="J186" t="n">
+        <v>3</v>
+      </c>
+      <c r="K186" t="n">
         <v>1</v>
       </c>
       <c r="L186" t="inlineStr">
@@ -13256,6 +13811,9 @@
         </is>
       </c>
       <c r="J187" t="n">
+        <v>3</v>
+      </c>
+      <c r="K187" t="n">
         <v>1</v>
       </c>
       <c r="L187" t="inlineStr">
@@ -13325,6 +13883,9 @@
         </is>
       </c>
       <c r="J188" t="n">
+        <v>3</v>
+      </c>
+      <c r="K188" t="n">
         <v>1</v>
       </c>
       <c r="L188" t="inlineStr">
@@ -13394,6 +13955,9 @@
         </is>
       </c>
       <c r="J189" t="n">
+        <v>3</v>
+      </c>
+      <c r="K189" t="n">
         <v>1</v>
       </c>
       <c r="L189" t="inlineStr">
@@ -13463,6 +14027,9 @@
         </is>
       </c>
       <c r="J190" t="n">
+        <v>3</v>
+      </c>
+      <c r="K190" t="n">
         <v>1</v>
       </c>
       <c r="L190" t="inlineStr">
@@ -13532,6 +14099,9 @@
         </is>
       </c>
       <c r="J191" t="n">
+        <v>3</v>
+      </c>
+      <c r="K191" t="n">
         <v>1</v>
       </c>
       <c r="L191" t="inlineStr">
@@ -13601,6 +14171,9 @@
         </is>
       </c>
       <c r="J192" t="n">
+        <v>3</v>
+      </c>
+      <c r="K192" t="n">
         <v>1</v>
       </c>
       <c r="L192" t="inlineStr">
@@ -13670,6 +14243,9 @@
         </is>
       </c>
       <c r="J193" t="n">
+        <v>3</v>
+      </c>
+      <c r="K193" t="n">
         <v>1</v>
       </c>
       <c r="L193" t="inlineStr">
@@ -13739,6 +14315,9 @@
         </is>
       </c>
       <c r="J194" t="n">
+        <v>3</v>
+      </c>
+      <c r="K194" t="n">
         <v>1</v>
       </c>
       <c r="L194" t="inlineStr">
@@ -13808,6 +14387,9 @@
         </is>
       </c>
       <c r="J195" t="n">
+        <v>3</v>
+      </c>
+      <c r="K195" t="n">
         <v>1</v>
       </c>
       <c r="L195" t="inlineStr">
@@ -13877,6 +14459,9 @@
         </is>
       </c>
       <c r="J196" t="n">
+        <v>3</v>
+      </c>
+      <c r="K196" t="n">
         <v>1</v>
       </c>
       <c r="L196" t="inlineStr">
@@ -13946,6 +14531,9 @@
         </is>
       </c>
       <c r="J197" t="n">
+        <v>3</v>
+      </c>
+      <c r="K197" t="n">
         <v>1</v>
       </c>
       <c r="L197" t="inlineStr">
@@ -14015,6 +14603,9 @@
         </is>
       </c>
       <c r="J198" t="n">
+        <v>3</v>
+      </c>
+      <c r="K198" t="n">
         <v>1</v>
       </c>
       <c r="L198" t="inlineStr">
@@ -14084,6 +14675,9 @@
         </is>
       </c>
       <c r="J199" t="n">
+        <v>3</v>
+      </c>
+      <c r="K199" t="n">
         <v>1</v>
       </c>
       <c r="L199" t="inlineStr">
@@ -14153,6 +14747,9 @@
         </is>
       </c>
       <c r="J200" t="n">
+        <v>3</v>
+      </c>
+      <c r="K200" t="n">
         <v>1</v>
       </c>
       <c r="L200" t="inlineStr">
@@ -14222,6 +14819,9 @@
         </is>
       </c>
       <c r="J201" t="n">
+        <v>3</v>
+      </c>
+      <c r="K201" t="n">
         <v>1</v>
       </c>
       <c r="L201" t="inlineStr">
@@ -14291,6 +14891,9 @@
         </is>
       </c>
       <c r="J202" t="n">
+        <v>3</v>
+      </c>
+      <c r="K202" t="n">
         <v>1</v>
       </c>
       <c r="L202" t="inlineStr">
@@ -14360,6 +14963,9 @@
         </is>
       </c>
       <c r="J203" t="n">
+        <v>3</v>
+      </c>
+      <c r="K203" t="n">
         <v>1</v>
       </c>
       <c r="L203" t="inlineStr">
@@ -14429,6 +15035,9 @@
         </is>
       </c>
       <c r="J204" t="n">
+        <v>3</v>
+      </c>
+      <c r="K204" t="n">
         <v>1</v>
       </c>
       <c r="L204" t="inlineStr">
@@ -14498,6 +15107,9 @@
         </is>
       </c>
       <c r="J205" t="n">
+        <v>3</v>
+      </c>
+      <c r="K205" t="n">
         <v>1</v>
       </c>
       <c r="L205" t="inlineStr">
@@ -14567,6 +15179,9 @@
         </is>
       </c>
       <c r="J206" t="n">
+        <v>3</v>
+      </c>
+      <c r="K206" t="n">
         <v>1</v>
       </c>
       <c r="L206" t="inlineStr">
@@ -14636,6 +15251,9 @@
         </is>
       </c>
       <c r="J207" t="n">
+        <v>3</v>
+      </c>
+      <c r="K207" t="n">
         <v>1</v>
       </c>
       <c r="L207" t="inlineStr">
@@ -14705,6 +15323,9 @@
         </is>
       </c>
       <c r="J208" t="n">
+        <v>3</v>
+      </c>
+      <c r="K208" t="n">
         <v>1</v>
       </c>
       <c r="L208" t="inlineStr">
@@ -14774,6 +15395,9 @@
         </is>
       </c>
       <c r="J209" t="n">
+        <v>3</v>
+      </c>
+      <c r="K209" t="n">
         <v>1</v>
       </c>
       <c r="L209" t="inlineStr">
@@ -14843,6 +15467,9 @@
         </is>
       </c>
       <c r="J210" t="n">
+        <v>3</v>
+      </c>
+      <c r="K210" t="n">
         <v>1</v>
       </c>
       <c r="L210" t="inlineStr">
@@ -14912,6 +15539,9 @@
         </is>
       </c>
       <c r="J211" t="n">
+        <v>3</v>
+      </c>
+      <c r="K211" t="n">
         <v>1</v>
       </c>
       <c r="L211" t="inlineStr">
@@ -14981,6 +15611,9 @@
         </is>
       </c>
       <c r="J212" t="n">
+        <v>3</v>
+      </c>
+      <c r="K212" t="n">
         <v>1</v>
       </c>
       <c r="L212" t="inlineStr">
@@ -15050,6 +15683,9 @@
         </is>
       </c>
       <c r="J213" t="n">
+        <v>3</v>
+      </c>
+      <c r="K213" t="n">
         <v>1</v>
       </c>
       <c r="L213" t="inlineStr">
@@ -15119,6 +15755,9 @@
         </is>
       </c>
       <c r="J214" t="n">
+        <v>3</v>
+      </c>
+      <c r="K214" t="n">
         <v>1</v>
       </c>
       <c r="L214" t="inlineStr">
@@ -15188,6 +15827,9 @@
         </is>
       </c>
       <c r="J215" t="n">
+        <v>3</v>
+      </c>
+      <c r="K215" t="n">
         <v>1</v>
       </c>
       <c r="L215" t="inlineStr">
@@ -15257,6 +15899,9 @@
         </is>
       </c>
       <c r="J216" t="n">
+        <v>3</v>
+      </c>
+      <c r="K216" t="n">
         <v>1</v>
       </c>
       <c r="L216" t="inlineStr">
@@ -15326,6 +15971,9 @@
         </is>
       </c>
       <c r="J217" t="n">
+        <v>3</v>
+      </c>
+      <c r="K217" t="n">
         <v>1</v>
       </c>
       <c r="L217" t="inlineStr">
@@ -15395,6 +16043,9 @@
         </is>
       </c>
       <c r="J218" t="n">
+        <v>3</v>
+      </c>
+      <c r="K218" t="n">
         <v>1</v>
       </c>
       <c r="L218" t="inlineStr">
@@ -15464,6 +16115,9 @@
         </is>
       </c>
       <c r="J219" t="n">
+        <v>3</v>
+      </c>
+      <c r="K219" t="n">
         <v>2</v>
       </c>
       <c r="L219" t="inlineStr">
@@ -15533,6 +16187,9 @@
         </is>
       </c>
       <c r="J220" t="n">
+        <v>3</v>
+      </c>
+      <c r="K220" t="n">
         <v>2</v>
       </c>
       <c r="L220" t="inlineStr">
@@ -15602,6 +16259,9 @@
         </is>
       </c>
       <c r="J221" t="n">
+        <v>3</v>
+      </c>
+      <c r="K221" t="n">
         <v>2</v>
       </c>
       <c r="L221" t="inlineStr">
@@ -15671,6 +16331,9 @@
         </is>
       </c>
       <c r="J222" t="n">
+        <v>3</v>
+      </c>
+      <c r="K222" t="n">
         <v>2</v>
       </c>
       <c r="L222" t="inlineStr">
@@ -15740,6 +16403,9 @@
         </is>
       </c>
       <c r="J223" t="n">
+        <v>3</v>
+      </c>
+      <c r="K223" t="n">
         <v>2</v>
       </c>
       <c r="L223" t="inlineStr">
@@ -15809,6 +16475,9 @@
         </is>
       </c>
       <c r="J224" t="n">
+        <v>3</v>
+      </c>
+      <c r="K224" t="n">
         <v>2</v>
       </c>
       <c r="L224" t="inlineStr">
@@ -15878,6 +16547,9 @@
         </is>
       </c>
       <c r="J225" t="n">
+        <v>3</v>
+      </c>
+      <c r="K225" t="n">
         <v>2</v>
       </c>
       <c r="L225" t="inlineStr">
@@ -15947,6 +16619,9 @@
         </is>
       </c>
       <c r="J226" t="n">
+        <v>3</v>
+      </c>
+      <c r="K226" t="n">
         <v>2</v>
       </c>
       <c r="L226" t="inlineStr">
@@ -16016,6 +16691,9 @@
         </is>
       </c>
       <c r="J227" t="n">
+        <v>3</v>
+      </c>
+      <c r="K227" t="n">
         <v>2</v>
       </c>
       <c r="L227" t="inlineStr">
@@ -16085,6 +16763,9 @@
         </is>
       </c>
       <c r="J228" t="n">
+        <v>3</v>
+      </c>
+      <c r="K228" t="n">
         <v>2</v>
       </c>
       <c r="L228" t="inlineStr">
@@ -16154,6 +16835,9 @@
         </is>
       </c>
       <c r="J229" t="n">
+        <v>3</v>
+      </c>
+      <c r="K229" t="n">
         <v>2</v>
       </c>
       <c r="L229" t="inlineStr">
@@ -16223,6 +16907,9 @@
         </is>
       </c>
       <c r="J230" t="n">
+        <v>3</v>
+      </c>
+      <c r="K230" t="n">
         <v>2</v>
       </c>
       <c r="L230" t="inlineStr">
@@ -16292,6 +16979,9 @@
         </is>
       </c>
       <c r="J231" t="n">
+        <v>3</v>
+      </c>
+      <c r="K231" t="n">
         <v>2</v>
       </c>
       <c r="L231" t="inlineStr">
@@ -16361,6 +17051,9 @@
         </is>
       </c>
       <c r="J232" t="n">
+        <v>3</v>
+      </c>
+      <c r="K232" t="n">
         <v>2</v>
       </c>
       <c r="L232" t="inlineStr">
@@ -16430,6 +17123,9 @@
         </is>
       </c>
       <c r="J233" t="n">
+        <v>3</v>
+      </c>
+      <c r="K233" t="n">
         <v>2</v>
       </c>
       <c r="L233" t="inlineStr">
@@ -16499,6 +17195,9 @@
         </is>
       </c>
       <c r="J234" t="n">
+        <v>3</v>
+      </c>
+      <c r="K234" t="n">
         <v>2</v>
       </c>
       <c r="L234" t="inlineStr">
@@ -16568,6 +17267,9 @@
         </is>
       </c>
       <c r="J235" t="n">
+        <v>3</v>
+      </c>
+      <c r="K235" t="n">
         <v>2</v>
       </c>
       <c r="L235" t="inlineStr">
@@ -16637,6 +17339,9 @@
         </is>
       </c>
       <c r="J236" t="n">
+        <v>3</v>
+      </c>
+      <c r="K236" t="n">
         <v>2</v>
       </c>
       <c r="L236" t="inlineStr">
@@ -16706,6 +17411,9 @@
         </is>
       </c>
       <c r="J237" t="n">
+        <v>3</v>
+      </c>
+      <c r="K237" t="n">
         <v>2</v>
       </c>
       <c r="L237" t="inlineStr">
@@ -16775,6 +17483,9 @@
         </is>
       </c>
       <c r="J238" t="n">
+        <v>3</v>
+      </c>
+      <c r="K238" t="n">
         <v>2</v>
       </c>
       <c r="L238" t="inlineStr">
@@ -16844,6 +17555,9 @@
         </is>
       </c>
       <c r="J239" t="n">
+        <v>3</v>
+      </c>
+      <c r="K239" t="n">
         <v>2</v>
       </c>
       <c r="L239" t="inlineStr">
@@ -16913,6 +17627,9 @@
         </is>
       </c>
       <c r="J240" t="n">
+        <v>3</v>
+      </c>
+      <c r="K240" t="n">
         <v>2</v>
       </c>
       <c r="L240" t="inlineStr">
@@ -16982,6 +17699,9 @@
         </is>
       </c>
       <c r="J241" t="n">
+        <v>3</v>
+      </c>
+      <c r="K241" t="n">
         <v>2</v>
       </c>
       <c r="L241" t="inlineStr">
@@ -17051,6 +17771,9 @@
         </is>
       </c>
       <c r="J242" t="n">
+        <v>3</v>
+      </c>
+      <c r="K242" t="n">
         <v>2</v>
       </c>
       <c r="L242" t="inlineStr">
@@ -17120,6 +17843,9 @@
         </is>
       </c>
       <c r="J243" t="n">
+        <v>3</v>
+      </c>
+      <c r="K243" t="n">
         <v>2</v>
       </c>
       <c r="L243" t="inlineStr">
@@ -17189,6 +17915,9 @@
         </is>
       </c>
       <c r="J244" t="n">
+        <v>3</v>
+      </c>
+      <c r="K244" t="n">
         <v>2</v>
       </c>
       <c r="L244" t="inlineStr">
@@ -17258,6 +17987,9 @@
         </is>
       </c>
       <c r="J245" t="n">
+        <v>3</v>
+      </c>
+      <c r="K245" t="n">
         <v>2</v>
       </c>
       <c r="L245" t="inlineStr">
@@ -17327,6 +18059,9 @@
         </is>
       </c>
       <c r="J246" t="n">
+        <v>3</v>
+      </c>
+      <c r="K246" t="n">
         <v>2</v>
       </c>
       <c r="L246" t="inlineStr">
@@ -17396,6 +18131,9 @@
         </is>
       </c>
       <c r="J247" t="n">
+        <v>3</v>
+      </c>
+      <c r="K247" t="n">
         <v>2</v>
       </c>
       <c r="L247" t="inlineStr">
@@ -17465,6 +18203,9 @@
         </is>
       </c>
       <c r="J248" t="n">
+        <v>3</v>
+      </c>
+      <c r="K248" t="n">
         <v>2</v>
       </c>
       <c r="L248" t="inlineStr">
@@ -17534,6 +18275,9 @@
         </is>
       </c>
       <c r="J249" t="n">
+        <v>3</v>
+      </c>
+      <c r="K249" t="n">
         <v>2</v>
       </c>
       <c r="L249" t="inlineStr">
@@ -17603,6 +18347,9 @@
         </is>
       </c>
       <c r="J250" t="n">
+        <v>3</v>
+      </c>
+      <c r="K250" t="n">
         <v>2</v>
       </c>
       <c r="L250" t="inlineStr">
@@ -17672,6 +18419,9 @@
         </is>
       </c>
       <c r="J251" t="n">
+        <v>3</v>
+      </c>
+      <c r="K251" t="n">
         <v>2</v>
       </c>
       <c r="L251" t="inlineStr">
@@ -17741,6 +18491,9 @@
         </is>
       </c>
       <c r="J252" t="n">
+        <v>3</v>
+      </c>
+      <c r="K252" t="n">
         <v>2</v>
       </c>
       <c r="L252" t="inlineStr">
@@ -17810,6 +18563,9 @@
         </is>
       </c>
       <c r="J253" t="n">
+        <v>3</v>
+      </c>
+      <c r="K253" t="n">
         <v>2</v>
       </c>
       <c r="L253" t="inlineStr">
@@ -17879,6 +18635,9 @@
         </is>
       </c>
       <c r="J254" t="n">
+        <v>3</v>
+      </c>
+      <c r="K254" t="n">
         <v>2</v>
       </c>
       <c r="L254" t="inlineStr">
@@ -17948,6 +18707,9 @@
         </is>
       </c>
       <c r="J255" t="n">
+        <v>3</v>
+      </c>
+      <c r="K255" t="n">
         <v>2</v>
       </c>
       <c r="L255" t="inlineStr">
@@ -18017,6 +18779,9 @@
         </is>
       </c>
       <c r="J256" t="n">
+        <v>3</v>
+      </c>
+      <c r="K256" t="n">
         <v>2</v>
       </c>
       <c r="L256" t="inlineStr">
@@ -18086,6 +18851,9 @@
         </is>
       </c>
       <c r="J257" t="n">
+        <v>4</v>
+      </c>
+      <c r="K257" t="n">
         <v>2</v>
       </c>
       <c r="L257" t="inlineStr">
@@ -18155,6 +18923,9 @@
         </is>
       </c>
       <c r="J258" t="n">
+        <v>4</v>
+      </c>
+      <c r="K258" t="n">
         <v>2</v>
       </c>
       <c r="L258" t="inlineStr">
@@ -18224,6 +18995,9 @@
         </is>
       </c>
       <c r="J259" t="n">
+        <v>4</v>
+      </c>
+      <c r="K259" t="n">
         <v>2</v>
       </c>
       <c r="L259" t="inlineStr">
@@ -18293,6 +19067,9 @@
         </is>
       </c>
       <c r="J260" t="n">
+        <v>4</v>
+      </c>
+      <c r="K260" t="n">
         <v>2</v>
       </c>
       <c r="L260" t="inlineStr">
@@ -18362,6 +19139,9 @@
         </is>
       </c>
       <c r="J261" t="n">
+        <v>4</v>
+      </c>
+      <c r="K261" t="n">
         <v>2</v>
       </c>
       <c r="L261" t="inlineStr">
@@ -18431,6 +19211,9 @@
         </is>
       </c>
       <c r="J262" t="n">
+        <v>4</v>
+      </c>
+      <c r="K262" t="n">
         <v>1</v>
       </c>
       <c r="L262" t="inlineStr">
@@ -18500,6 +19283,9 @@
         </is>
       </c>
       <c r="J263" t="n">
+        <v>4</v>
+      </c>
+      <c r="K263" t="n">
         <v>1</v>
       </c>
       <c r="L263" t="inlineStr">
@@ -18569,6 +19355,9 @@
         </is>
       </c>
       <c r="J264" t="n">
+        <v>4</v>
+      </c>
+      <c r="K264" t="n">
         <v>1</v>
       </c>
       <c r="L264" t="inlineStr">
@@ -18638,6 +19427,9 @@
         </is>
       </c>
       <c r="J265" t="n">
+        <v>4</v>
+      </c>
+      <c r="K265" t="n">
         <v>1</v>
       </c>
       <c r="L265" t="inlineStr">
@@ -18707,6 +19499,9 @@
         </is>
       </c>
       <c r="J266" t="n">
+        <v>4</v>
+      </c>
+      <c r="K266" t="n">
         <v>1</v>
       </c>
       <c r="L266" t="inlineStr">
@@ -18776,6 +19571,9 @@
         </is>
       </c>
       <c r="J267" t="n">
+        <v>4</v>
+      </c>
+      <c r="K267" t="n">
         <v>1</v>
       </c>
       <c r="L267" t="inlineStr">
@@ -18845,6 +19643,9 @@
         </is>
       </c>
       <c r="J268" t="n">
+        <v>4</v>
+      </c>
+      <c r="K268" t="n">
         <v>1</v>
       </c>
       <c r="L268" t="inlineStr">
@@ -18914,6 +19715,9 @@
         </is>
       </c>
       <c r="J269" t="n">
+        <v>4</v>
+      </c>
+      <c r="K269" t="n">
         <v>1</v>
       </c>
       <c r="L269" t="inlineStr">
@@ -18983,6 +19787,9 @@
         </is>
       </c>
       <c r="J270" t="n">
+        <v>4</v>
+      </c>
+      <c r="K270" t="n">
         <v>1</v>
       </c>
       <c r="L270" t="inlineStr">
@@ -19052,6 +19859,9 @@
         </is>
       </c>
       <c r="J271" t="n">
+        <v>4</v>
+      </c>
+      <c r="K271" t="n">
         <v>1</v>
       </c>
       <c r="L271" t="inlineStr">
@@ -19121,6 +19931,9 @@
         </is>
       </c>
       <c r="J272" t="n">
+        <v>4</v>
+      </c>
+      <c r="K272" t="n">
         <v>2</v>
       </c>
       <c r="L272" t="inlineStr">
@@ -19190,6 +20003,9 @@
         </is>
       </c>
       <c r="J273" t="n">
+        <v>4</v>
+      </c>
+      <c r="K273" t="n">
         <v>2</v>
       </c>
       <c r="L273" t="inlineStr">
@@ -19259,6 +20075,9 @@
         </is>
       </c>
       <c r="J274" t="n">
+        <v>4</v>
+      </c>
+      <c r="K274" t="n">
         <v>2</v>
       </c>
       <c r="L274" t="inlineStr">
@@ -19328,6 +20147,9 @@
         </is>
       </c>
       <c r="J275" t="n">
+        <v>4</v>
+      </c>
+      <c r="K275" t="n">
         <v>2</v>
       </c>
       <c r="L275" t="inlineStr">
@@ -19397,6 +20219,9 @@
         </is>
       </c>
       <c r="J276" t="n">
+        <v>4</v>
+      </c>
+      <c r="K276" t="n">
         <v>2</v>
       </c>
       <c r="L276" t="inlineStr">
@@ -19466,6 +20291,9 @@
         </is>
       </c>
       <c r="J277" t="n">
+        <v>4</v>
+      </c>
+      <c r="K277" t="n">
         <v>2</v>
       </c>
       <c r="L277" t="inlineStr">
@@ -19535,6 +20363,9 @@
         </is>
       </c>
       <c r="J278" t="n">
+        <v>4</v>
+      </c>
+      <c r="K278" t="n">
         <v>2</v>
       </c>
       <c r="L278" t="inlineStr">
@@ -19604,6 +20435,9 @@
         </is>
       </c>
       <c r="J279" t="n">
+        <v>4</v>
+      </c>
+      <c r="K279" t="n">
         <v>2</v>
       </c>
       <c r="L279" t="inlineStr">
@@ -19673,6 +20507,9 @@
         </is>
       </c>
       <c r="J280" t="n">
+        <v>4</v>
+      </c>
+      <c r="K280" t="n">
         <v>2</v>
       </c>
       <c r="L280" t="inlineStr">
@@ -19742,6 +20579,9 @@
         </is>
       </c>
       <c r="J281" t="n">
+        <v>4</v>
+      </c>
+      <c r="K281" t="n">
         <v>2</v>
       </c>
       <c r="L281" t="inlineStr">
@@ -19811,6 +20651,9 @@
         </is>
       </c>
       <c r="J282" t="n">
+        <v>4</v>
+      </c>
+      <c r="K282" t="n">
         <v>2</v>
       </c>
       <c r="L282" t="inlineStr">
@@ -19880,6 +20723,9 @@
         </is>
       </c>
       <c r="J283" t="n">
+        <v>4</v>
+      </c>
+      <c r="K283" t="n">
         <v>2</v>
       </c>
       <c r="L283" t="inlineStr">
@@ -19949,6 +20795,9 @@
         </is>
       </c>
       <c r="J284" t="n">
+        <v>4</v>
+      </c>
+      <c r="K284" t="n">
         <v>2</v>
       </c>
       <c r="L284" t="inlineStr">
@@ -20018,6 +20867,9 @@
         </is>
       </c>
       <c r="J285" t="n">
+        <v>4</v>
+      </c>
+      <c r="K285" t="n">
         <v>2</v>
       </c>
       <c r="L285" t="inlineStr">
@@ -20087,6 +20939,9 @@
         </is>
       </c>
       <c r="J286" t="n">
+        <v>4</v>
+      </c>
+      <c r="K286" t="n">
         <v>2</v>
       </c>
       <c r="L286" t="inlineStr">
@@ -20156,6 +21011,9 @@
         </is>
       </c>
       <c r="J287" t="n">
+        <v>4</v>
+      </c>
+      <c r="K287" t="n">
         <v>2</v>
       </c>
       <c r="L287" t="inlineStr">
@@ -20225,6 +21083,9 @@
         </is>
       </c>
       <c r="J288" t="n">
+        <v>3</v>
+      </c>
+      <c r="K288" t="n">
         <v>2</v>
       </c>
       <c r="L288" t="inlineStr">
@@ -20294,6 +21155,9 @@
         </is>
       </c>
       <c r="J289" t="n">
+        <v>3</v>
+      </c>
+      <c r="K289" t="n">
         <v>2</v>
       </c>
       <c r="L289" t="inlineStr">
@@ -20363,6 +21227,9 @@
         </is>
       </c>
       <c r="J290" t="n">
+        <v>3</v>
+      </c>
+      <c r="K290" t="n">
         <v>2</v>
       </c>
       <c r="L290" t="inlineStr">
@@ -20432,6 +21299,9 @@
         </is>
       </c>
       <c r="J291" t="n">
+        <v>3</v>
+      </c>
+      <c r="K291" t="n">
         <v>2</v>
       </c>
       <c r="L291" t="inlineStr">
@@ -20501,6 +21371,9 @@
         </is>
       </c>
       <c r="J292" t="n">
+        <v>3</v>
+      </c>
+      <c r="K292" t="n">
         <v>2</v>
       </c>
       <c r="L292" t="inlineStr">
@@ -20570,6 +21443,9 @@
         </is>
       </c>
       <c r="J293" t="n">
+        <v>3</v>
+      </c>
+      <c r="K293" t="n">
         <v>2</v>
       </c>
       <c r="L293" t="inlineStr">
@@ -20639,6 +21515,9 @@
         </is>
       </c>
       <c r="J294" t="n">
+        <v>4</v>
+      </c>
+      <c r="K294" t="n">
         <v>1</v>
       </c>
       <c r="L294" t="inlineStr">
@@ -20708,6 +21587,9 @@
         </is>
       </c>
       <c r="J295" t="n">
+        <v>4</v>
+      </c>
+      <c r="K295" t="n">
         <v>1</v>
       </c>
       <c r="L295" t="inlineStr">
@@ -20777,6 +21659,9 @@
         </is>
       </c>
       <c r="J296" t="n">
+        <v>4</v>
+      </c>
+      <c r="K296" t="n">
         <v>1</v>
       </c>
       <c r="L296" t="inlineStr">
@@ -20846,6 +21731,9 @@
         </is>
       </c>
       <c r="J297" t="n">
+        <v>4</v>
+      </c>
+      <c r="K297" t="n">
         <v>1</v>
       </c>
       <c r="L297" t="inlineStr">
@@ -20915,6 +21803,9 @@
         </is>
       </c>
       <c r="J298" t="n">
+        <v>4</v>
+      </c>
+      <c r="K298" t="n">
         <v>1</v>
       </c>
       <c r="L298" t="inlineStr">
@@ -20984,6 +21875,9 @@
         </is>
       </c>
       <c r="J299" t="n">
+        <v>4</v>
+      </c>
+      <c r="K299" t="n">
         <v>1</v>
       </c>
       <c r="L299" t="inlineStr">
@@ -21053,6 +21947,9 @@
         </is>
       </c>
       <c r="J300" t="n">
+        <v>4</v>
+      </c>
+      <c r="K300" t="n">
         <v>1</v>
       </c>
       <c r="L300" t="inlineStr">
@@ -21122,6 +22019,9 @@
         </is>
       </c>
       <c r="J301" t="n">
+        <v>4</v>
+      </c>
+      <c r="K301" t="n">
         <v>1</v>
       </c>
       <c r="L301" t="inlineStr">
@@ -21191,6 +22091,9 @@
         </is>
       </c>
       <c r="J302" t="n">
+        <v>4</v>
+      </c>
+      <c r="K302" t="n">
         <v>1</v>
       </c>
       <c r="L302" t="inlineStr">
@@ -21260,6 +22163,9 @@
         </is>
       </c>
       <c r="J303" t="n">
+        <v>4</v>
+      </c>
+      <c r="K303" t="n">
         <v>2</v>
       </c>
       <c r="L303" t="inlineStr">
@@ -21329,6 +22235,9 @@
         </is>
       </c>
       <c r="J304" t="n">
+        <v>4</v>
+      </c>
+      <c r="K304" t="n">
         <v>2</v>
       </c>
       <c r="L304" t="inlineStr">
@@ -21398,6 +22307,9 @@
         </is>
       </c>
       <c r="J305" t="n">
+        <v>4</v>
+      </c>
+      <c r="K305" t="n">
         <v>2</v>
       </c>
       <c r="L305" t="inlineStr">
@@ -21467,6 +22379,9 @@
         </is>
       </c>
       <c r="J306" t="n">
+        <v>4</v>
+      </c>
+      <c r="K306" t="n">
         <v>2</v>
       </c>
       <c r="L306" t="inlineStr">
@@ -21536,6 +22451,9 @@
         </is>
       </c>
       <c r="J307" t="n">
+        <v>4</v>
+      </c>
+      <c r="K307" t="n">
         <v>2</v>
       </c>
       <c r="L307" t="inlineStr">
@@ -21605,6 +22523,9 @@
         </is>
       </c>
       <c r="J308" t="n">
+        <v>4</v>
+      </c>
+      <c r="K308" t="n">
         <v>2</v>
       </c>
       <c r="L308" t="inlineStr">
@@ -21674,6 +22595,9 @@
         </is>
       </c>
       <c r="J309" t="n">
+        <v>4</v>
+      </c>
+      <c r="K309" t="n">
         <v>2</v>
       </c>
       <c r="L309" t="inlineStr">
@@ -21743,6 +22667,9 @@
         </is>
       </c>
       <c r="J310" t="n">
+        <v>4</v>
+      </c>
+      <c r="K310" t="n">
         <v>2</v>
       </c>
       <c r="L310" t="inlineStr">
@@ -21812,6 +22739,9 @@
         </is>
       </c>
       <c r="J311" t="n">
+        <v>4</v>
+      </c>
+      <c r="K311" t="n">
         <v>2</v>
       </c>
       <c r="L311" t="inlineStr">
@@ -21881,6 +22811,9 @@
         </is>
       </c>
       <c r="J312" t="n">
+        <v>3</v>
+      </c>
+      <c r="K312" t="n">
         <v>2</v>
       </c>
       <c r="L312" t="inlineStr">
@@ -21950,6 +22883,9 @@
         </is>
       </c>
       <c r="J313" t="n">
+        <v>3</v>
+      </c>
+      <c r="K313" t="n">
         <v>2</v>
       </c>
       <c r="L313" t="inlineStr">
@@ -22019,6 +22955,9 @@
         </is>
       </c>
       <c r="J314" t="n">
+        <v>3</v>
+      </c>
+      <c r="K314" t="n">
         <v>2</v>
       </c>
       <c r="L314" t="inlineStr">
@@ -22088,6 +23027,9 @@
         </is>
       </c>
       <c r="J315" t="n">
+        <v>4</v>
+      </c>
+      <c r="K315" t="n">
         <v>1</v>
       </c>
       <c r="L315" t="inlineStr">
@@ -22157,6 +23099,9 @@
         </is>
       </c>
       <c r="J316" t="n">
+        <v>4</v>
+      </c>
+      <c r="K316" t="n">
         <v>1</v>
       </c>
       <c r="L316" t="inlineStr">
@@ -22226,6 +23171,9 @@
         </is>
       </c>
       <c r="J317" t="n">
+        <v>4</v>
+      </c>
+      <c r="K317" t="n">
         <v>1</v>
       </c>
       <c r="L317" t="inlineStr">
@@ -22295,6 +23243,9 @@
         </is>
       </c>
       <c r="J318" t="n">
+        <v>4</v>
+      </c>
+      <c r="K318" t="n">
         <v>1</v>
       </c>
       <c r="L318" t="inlineStr">
@@ -22364,6 +23315,9 @@
         </is>
       </c>
       <c r="J319" t="n">
+        <v>4</v>
+      </c>
+      <c r="K319" t="n">
         <v>1</v>
       </c>
       <c r="L319" t="inlineStr">
@@ -22433,6 +23387,9 @@
         </is>
       </c>
       <c r="J320" t="n">
+        <v>4</v>
+      </c>
+      <c r="K320" t="n">
         <v>1</v>
       </c>
       <c r="L320" t="inlineStr">
@@ -22502,6 +23459,9 @@
         </is>
       </c>
       <c r="J321" t="n">
+        <v>4</v>
+      </c>
+      <c r="K321" t="n">
         <v>2</v>
       </c>
       <c r="L321" t="inlineStr">
@@ -22571,6 +23531,9 @@
         </is>
       </c>
       <c r="J322" t="n">
+        <v>4</v>
+      </c>
+      <c r="K322" t="n">
         <v>2</v>
       </c>
       <c r="L322" t="inlineStr">
@@ -22640,6 +23603,9 @@
         </is>
       </c>
       <c r="J323" t="n">
+        <v>4</v>
+      </c>
+      <c r="K323" t="n">
         <v>2</v>
       </c>
       <c r="L323" t="inlineStr">
@@ -22709,6 +23675,9 @@
         </is>
       </c>
       <c r="J324" t="n">
+        <v>4</v>
+      </c>
+      <c r="K324" t="n">
         <v>2</v>
       </c>
       <c r="L324" t="inlineStr">
@@ -22778,6 +23747,9 @@
         </is>
       </c>
       <c r="J325" t="n">
+        <v>4</v>
+      </c>
+      <c r="K325" t="n">
         <v>2</v>
       </c>
       <c r="L325" t="inlineStr">
@@ -22847,6 +23819,9 @@
         </is>
       </c>
       <c r="J326" t="n">
+        <v>4</v>
+      </c>
+      <c r="K326" t="n">
         <v>2</v>
       </c>
       <c r="L326" t="inlineStr">
@@ -22916,6 +23891,9 @@
         </is>
       </c>
       <c r="J327" t="n">
+        <v>4</v>
+      </c>
+      <c r="K327" t="n">
         <v>2</v>
       </c>
       <c r="L327" t="inlineStr">
@@ -22985,6 +23963,9 @@
         </is>
       </c>
       <c r="J328" t="n">
+        <v>4</v>
+      </c>
+      <c r="K328" t="n">
         <v>2</v>
       </c>
       <c r="L328" t="inlineStr">
@@ -23054,6 +24035,9 @@
         </is>
       </c>
       <c r="J329" t="n">
+        <v>4</v>
+      </c>
+      <c r="K329" t="n">
         <v>2</v>
       </c>
       <c r="L329" t="inlineStr">
@@ -23123,6 +24107,9 @@
         </is>
       </c>
       <c r="J330" t="n">
+        <v>3</v>
+      </c>
+      <c r="K330" t="n">
         <v>2</v>
       </c>
       <c r="L330" t="inlineStr">
@@ -23192,6 +24179,9 @@
         </is>
       </c>
       <c r="J331" t="n">
+        <v>3</v>
+      </c>
+      <c r="K331" t="n">
         <v>2</v>
       </c>
       <c r="L331" t="inlineStr">
@@ -23261,6 +24251,9 @@
         </is>
       </c>
       <c r="J332" t="n">
+        <v>3</v>
+      </c>
+      <c r="K332" t="n">
         <v>2</v>
       </c>
       <c r="L332" t="inlineStr">
@@ -23330,6 +24323,9 @@
         </is>
       </c>
       <c r="J333" t="n">
+        <v>3</v>
+      </c>
+      <c r="K333" t="n">
         <v>2</v>
       </c>
       <c r="L333" t="inlineStr">
@@ -23399,6 +24395,9 @@
         </is>
       </c>
       <c r="J334" t="n">
+        <v>3</v>
+      </c>
+      <c r="K334" t="n">
         <v>2</v>
       </c>
       <c r="L334" t="inlineStr">
@@ -23468,6 +24467,9 @@
         </is>
       </c>
       <c r="J335" t="n">
+        <v>4</v>
+      </c>
+      <c r="K335" t="n">
         <v>1</v>
       </c>
       <c r="L335" t="inlineStr">
@@ -23537,6 +24539,9 @@
         </is>
       </c>
       <c r="J336" t="n">
+        <v>4</v>
+      </c>
+      <c r="K336" t="n">
         <v>1</v>
       </c>
       <c r="L336" t="inlineStr">
@@ -23606,6 +24611,9 @@
         </is>
       </c>
       <c r="J337" t="n">
+        <v>4</v>
+      </c>
+      <c r="K337" t="n">
         <v>1</v>
       </c>
       <c r="L337" t="inlineStr">
@@ -23675,6 +24683,9 @@
         </is>
       </c>
       <c r="J338" t="n">
+        <v>4</v>
+      </c>
+      <c r="K338" t="n">
         <v>2</v>
       </c>
       <c r="L338" t="inlineStr">
@@ -23744,6 +24755,9 @@
         </is>
       </c>
       <c r="J339" t="n">
+        <v>4</v>
+      </c>
+      <c r="K339" t="n">
         <v>2</v>
       </c>
       <c r="L339" t="inlineStr">
@@ -23813,6 +24827,9 @@
         </is>
       </c>
       <c r="J340" t="n">
+        <v>4</v>
+      </c>
+      <c r="K340" t="n">
         <v>2</v>
       </c>
       <c r="L340" t="inlineStr">
@@ -23882,6 +24899,9 @@
         </is>
       </c>
       <c r="J341" t="n">
+        <v>3</v>
+      </c>
+      <c r="K341" t="n">
         <v>2</v>
       </c>
       <c r="L341" t="inlineStr">
@@ -23951,6 +24971,9 @@
         </is>
       </c>
       <c r="J342" t="n">
+        <v>3</v>
+      </c>
+      <c r="K342" t="n">
         <v>2</v>
       </c>
       <c r="L342" t="inlineStr">
@@ -24020,6 +25043,9 @@
         </is>
       </c>
       <c r="J343" t="n">
+        <v>3</v>
+      </c>
+      <c r="K343" t="n">
         <v>2</v>
       </c>
       <c r="L343" t="inlineStr">
@@ -24089,6 +25115,9 @@
         </is>
       </c>
       <c r="J344" t="n">
+        <v>3</v>
+      </c>
+      <c r="K344" t="n">
         <v>2</v>
       </c>
       <c r="L344" t="inlineStr">
@@ -24158,6 +25187,9 @@
         </is>
       </c>
       <c r="J345" t="n">
+        <v>3</v>
+      </c>
+      <c r="K345" t="n">
         <v>2</v>
       </c>
       <c r="L345" t="inlineStr">
@@ -24227,6 +25259,9 @@
         </is>
       </c>
       <c r="J346" t="n">
+        <v>3</v>
+      </c>
+      <c r="K346" t="n">
         <v>2</v>
       </c>
       <c r="L346" t="inlineStr">
@@ -24296,6 +25331,9 @@
         </is>
       </c>
       <c r="J347" t="n">
+        <v>4</v>
+      </c>
+      <c r="K347" t="n">
         <v>1</v>
       </c>
       <c r="L347" t="inlineStr">
@@ -24365,6 +25403,9 @@
         </is>
       </c>
       <c r="J348" t="n">
+        <v>4</v>
+      </c>
+      <c r="K348" t="n">
         <v>1</v>
       </c>
       <c r="L348" t="inlineStr">
@@ -24434,6 +25475,9 @@
         </is>
       </c>
       <c r="J349" t="n">
+        <v>4</v>
+      </c>
+      <c r="K349" t="n">
         <v>1</v>
       </c>
       <c r="L349" t="inlineStr">
@@ -24503,6 +25547,9 @@
         </is>
       </c>
       <c r="J350" t="n">
+        <v>4</v>
+      </c>
+      <c r="K350" t="n">
         <v>1</v>
       </c>
       <c r="L350" t="inlineStr">
@@ -24572,6 +25619,9 @@
         </is>
       </c>
       <c r="J351" t="n">
+        <v>4</v>
+      </c>
+      <c r="K351" t="n">
         <v>1</v>
       </c>
       <c r="L351" t="inlineStr">
@@ -24641,6 +25691,9 @@
         </is>
       </c>
       <c r="J352" t="n">
+        <v>4</v>
+      </c>
+      <c r="K352" t="n">
         <v>1</v>
       </c>
       <c r="L352" t="inlineStr">
@@ -24710,6 +25763,9 @@
         </is>
       </c>
       <c r="J353" t="n">
+        <v>4</v>
+      </c>
+      <c r="K353" t="n">
         <v>2</v>
       </c>
       <c r="L353" t="inlineStr">
@@ -24779,6 +25835,9 @@
         </is>
       </c>
       <c r="J354" t="n">
+        <v>4</v>
+      </c>
+      <c r="K354" t="n">
         <v>2</v>
       </c>
       <c r="L354" t="inlineStr">
@@ -24848,6 +25907,9 @@
         </is>
       </c>
       <c r="J355" t="n">
+        <v>4</v>
+      </c>
+      <c r="K355" t="n">
         <v>2</v>
       </c>
       <c r="L355" t="inlineStr">
@@ -24917,6 +25979,9 @@
         </is>
       </c>
       <c r="J356" t="n">
+        <v>4</v>
+      </c>
+      <c r="K356" t="n">
         <v>2</v>
       </c>
       <c r="L356" t="inlineStr">
@@ -24986,6 +26051,9 @@
         </is>
       </c>
       <c r="J357" t="n">
+        <v>4</v>
+      </c>
+      <c r="K357" t="n">
         <v>2</v>
       </c>
       <c r="L357" t="inlineStr">
@@ -25055,6 +26123,9 @@
         </is>
       </c>
       <c r="J358" t="n">
+        <v>4</v>
+      </c>
+      <c r="K358" t="n">
         <v>2</v>
       </c>
       <c r="L358" t="inlineStr">
@@ -25124,6 +26195,9 @@
         </is>
       </c>
       <c r="J359" t="n">
+        <v>4</v>
+      </c>
+      <c r="K359" t="n">
         <v>1</v>
       </c>
       <c r="L359" t="inlineStr">
@@ -25193,6 +26267,9 @@
         </is>
       </c>
       <c r="J360" t="n">
+        <v>4</v>
+      </c>
+      <c r="K360" t="n">
         <v>1</v>
       </c>
       <c r="L360" t="inlineStr">
@@ -25262,6 +26339,9 @@
         </is>
       </c>
       <c r="J361" t="n">
+        <v>4</v>
+      </c>
+      <c r="K361" t="n">
         <v>1</v>
       </c>
       <c r="L361" t="inlineStr">
@@ -25331,6 +26411,9 @@
         </is>
       </c>
       <c r="J362" t="n">
+        <v>4</v>
+      </c>
+      <c r="K362" t="n">
         <v>1</v>
       </c>
       <c r="L362" t="inlineStr">
@@ -25400,6 +26483,9 @@
         </is>
       </c>
       <c r="J363" t="n">
+        <v>4</v>
+      </c>
+      <c r="K363" t="n">
         <v>1</v>
       </c>
       <c r="L363" t="inlineStr">
@@ -25469,6 +26555,9 @@
         </is>
       </c>
       <c r="J364" t="n">
+        <v>4</v>
+      </c>
+      <c r="K364" t="n">
         <v>1</v>
       </c>
       <c r="L364" t="inlineStr">
@@ -25538,6 +26627,9 @@
         </is>
       </c>
       <c r="J365" t="n">
+        <v>4</v>
+      </c>
+      <c r="K365" t="n">
         <v>1</v>
       </c>
       <c r="L365" t="inlineStr">
@@ -25607,6 +26699,9 @@
         </is>
       </c>
       <c r="J366" t="n">
+        <v>4</v>
+      </c>
+      <c r="K366" t="n">
         <v>1</v>
       </c>
       <c r="L366" t="inlineStr">
@@ -25676,6 +26771,9 @@
         </is>
       </c>
       <c r="J367" t="n">
+        <v>4</v>
+      </c>
+      <c r="K367" t="n">
         <v>1</v>
       </c>
       <c r="L367" t="inlineStr">
@@ -25745,6 +26843,9 @@
         </is>
       </c>
       <c r="J368" t="n">
+        <v>4</v>
+      </c>
+      <c r="K368" t="n">
         <v>1</v>
       </c>
       <c r="L368" t="inlineStr">
@@ -25814,6 +26915,9 @@
         </is>
       </c>
       <c r="J369" t="n">
+        <v>4</v>
+      </c>
+      <c r="K369" t="n">
         <v>1</v>
       </c>
       <c r="L369" t="inlineStr">
@@ -25883,6 +26987,9 @@
         </is>
       </c>
       <c r="J370" t="n">
+        <v>4</v>
+      </c>
+      <c r="K370" t="n">
         <v>1</v>
       </c>
       <c r="L370" t="inlineStr">
@@ -25952,6 +27059,9 @@
         </is>
       </c>
       <c r="J371" t="n">
+        <v>4</v>
+      </c>
+      <c r="K371" t="n">
         <v>2</v>
       </c>
       <c r="L371" t="inlineStr">
@@ -26021,6 +27131,9 @@
         </is>
       </c>
       <c r="J372" t="n">
+        <v>2</v>
+      </c>
+      <c r="K372" t="n">
         <v>1</v>
       </c>
       <c r="L372" t="inlineStr">
@@ -26090,6 +27203,9 @@
         </is>
       </c>
       <c r="J373" t="n">
+        <v>2</v>
+      </c>
+      <c r="K373" t="n">
         <v>1</v>
       </c>
       <c r="L373" t="inlineStr">
@@ -26159,6 +27275,9 @@
         </is>
       </c>
       <c r="J374" t="n">
+        <v>2</v>
+      </c>
+      <c r="K374" t="n">
         <v>1</v>
       </c>
       <c r="L374" t="inlineStr">
@@ -26228,6 +27347,9 @@
         </is>
       </c>
       <c r="J375" t="n">
+        <v>2</v>
+      </c>
+      <c r="K375" t="n">
         <v>1</v>
       </c>
       <c r="L375" t="inlineStr">
@@ -26297,6 +27419,9 @@
         </is>
       </c>
       <c r="J376" t="n">
+        <v>1</v>
+      </c>
+      <c r="K376" t="n">
         <v>2</v>
       </c>
       <c r="L376" t="inlineStr">
@@ -26366,6 +27491,9 @@
         </is>
       </c>
       <c r="J377" t="n">
+        <v>1</v>
+      </c>
+      <c r="K377" t="n">
         <v>2</v>
       </c>
       <c r="L377" t="inlineStr">
@@ -26435,6 +27563,9 @@
         </is>
       </c>
       <c r="J378" t="n">
+        <v>1</v>
+      </c>
+      <c r="K378" t="n">
         <v>2</v>
       </c>
       <c r="L378" t="inlineStr">
@@ -26504,6 +27635,9 @@
         </is>
       </c>
       <c r="J379" t="n">
+        <v>1</v>
+      </c>
+      <c r="K379" t="n">
         <v>2</v>
       </c>
       <c r="L379" t="inlineStr">
@@ -26573,6 +27707,9 @@
         </is>
       </c>
       <c r="J380" t="n">
+        <v>1</v>
+      </c>
+      <c r="K380" t="n">
         <v>2</v>
       </c>
       <c r="L380" t="inlineStr">
@@ -26642,6 +27779,9 @@
         </is>
       </c>
       <c r="J381" t="n">
+        <v>1</v>
+      </c>
+      <c r="K381" t="n">
         <v>2</v>
       </c>
       <c r="L381" t="inlineStr">
@@ -26711,6 +27851,9 @@
         </is>
       </c>
       <c r="J382" t="n">
+        <v>1</v>
+      </c>
+      <c r="K382" t="n">
         <v>2</v>
       </c>
       <c r="L382" t="inlineStr">
@@ -26780,6 +27923,9 @@
         </is>
       </c>
       <c r="J383" t="n">
+        <v>1</v>
+      </c>
+      <c r="K383" t="n">
         <v>2</v>
       </c>
       <c r="L383" t="inlineStr">
@@ -26849,6 +27995,9 @@
         </is>
       </c>
       <c r="J384" t="n">
+        <v>1</v>
+      </c>
+      <c r="K384" t="n">
         <v>2</v>
       </c>
       <c r="L384" t="inlineStr">
@@ -26918,6 +28067,9 @@
         </is>
       </c>
       <c r="J385" t="n">
+        <v>1</v>
+      </c>
+      <c r="K385" t="n">
         <v>2</v>
       </c>
       <c r="L385" t="inlineStr">
@@ -26987,6 +28139,9 @@
         </is>
       </c>
       <c r="J386" t="n">
+        <v>1</v>
+      </c>
+      <c r="K386" t="n">
         <v>2</v>
       </c>
       <c r="L386" t="inlineStr">
@@ -27056,6 +28211,9 @@
         </is>
       </c>
       <c r="J387" t="n">
+        <v>1</v>
+      </c>
+      <c r="K387" t="n">
         <v>2</v>
       </c>
       <c r="L387" t="inlineStr">
@@ -27125,6 +28283,9 @@
         </is>
       </c>
       <c r="J388" t="n">
+        <v>1</v>
+      </c>
+      <c r="K388" t="n">
         <v>2</v>
       </c>
       <c r="L388" t="inlineStr">
@@ -27194,6 +28355,9 @@
         </is>
       </c>
       <c r="J389" t="n">
+        <v>1</v>
+      </c>
+      <c r="K389" t="n">
         <v>2</v>
       </c>
       <c r="L389" t="inlineStr">
@@ -27263,6 +28427,9 @@
         </is>
       </c>
       <c r="J390" t="n">
+        <v>1</v>
+      </c>
+      <c r="K390" t="n">
         <v>2</v>
       </c>
       <c r="L390" t="inlineStr">
@@ -27332,6 +28499,9 @@
         </is>
       </c>
       <c r="J391" t="n">
+        <v>1</v>
+      </c>
+      <c r="K391" t="n">
         <v>2</v>
       </c>
       <c r="L391" t="inlineStr">
@@ -27401,6 +28571,9 @@
         </is>
       </c>
       <c r="J392" t="n">
+        <v>1</v>
+      </c>
+      <c r="K392" t="n">
         <v>2</v>
       </c>
       <c r="L392" t="inlineStr">
@@ -27472,6 +28645,9 @@
       <c r="J393" t="n">
         <v>1</v>
       </c>
+      <c r="K393" t="n">
+        <v>1</v>
+      </c>
       <c r="L393" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -27541,6 +28717,9 @@
       <c r="J394" t="n">
         <v>1</v>
       </c>
+      <c r="K394" t="n">
+        <v>1</v>
+      </c>
       <c r="L394" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -27610,6 +28789,9 @@
       <c r="J395" t="n">
         <v>1</v>
       </c>
+      <c r="K395" t="n">
+        <v>1</v>
+      </c>
       <c r="L395" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -27679,6 +28861,9 @@
       <c r="J396" t="n">
         <v>1</v>
       </c>
+      <c r="K396" t="n">
+        <v>1</v>
+      </c>
       <c r="L396" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -27748,6 +28933,9 @@
       <c r="J397" t="n">
         <v>1</v>
       </c>
+      <c r="K397" t="n">
+        <v>1</v>
+      </c>
       <c r="L397" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -27817,6 +29005,9 @@
       <c r="J398" t="n">
         <v>1</v>
       </c>
+      <c r="K398" t="n">
+        <v>1</v>
+      </c>
       <c r="L398" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -27886,6 +29077,9 @@
       <c r="J399" t="n">
         <v>1</v>
       </c>
+      <c r="K399" t="n">
+        <v>1</v>
+      </c>
       <c r="L399" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -27955,6 +29149,9 @@
       <c r="J400" t="n">
         <v>1</v>
       </c>
+      <c r="K400" t="n">
+        <v>1</v>
+      </c>
       <c r="L400" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -28024,6 +29221,9 @@
       <c r="J401" t="n">
         <v>1</v>
       </c>
+      <c r="K401" t="n">
+        <v>1</v>
+      </c>
       <c r="L401" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -28093,6 +29293,9 @@
       <c r="J402" t="n">
         <v>1</v>
       </c>
+      <c r="K402" t="n">
+        <v>1</v>
+      </c>
       <c r="L402" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -28162,6 +29365,9 @@
       <c r="J403" t="n">
         <v>1</v>
       </c>
+      <c r="K403" t="n">
+        <v>1</v>
+      </c>
       <c r="L403" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -28231,6 +29437,9 @@
       <c r="J404" t="n">
         <v>1</v>
       </c>
+      <c r="K404" t="n">
+        <v>1</v>
+      </c>
       <c r="L404" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -28300,6 +29509,9 @@
       <c r="J405" t="n">
         <v>1</v>
       </c>
+      <c r="K405" t="n">
+        <v>1</v>
+      </c>
       <c r="L405" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -28369,6 +29581,9 @@
       <c r="J406" t="n">
         <v>1</v>
       </c>
+      <c r="K406" t="n">
+        <v>1</v>
+      </c>
       <c r="L406" t="inlineStr">
         <is>
           <t>Rama</t>
@@ -28436,6 +29651,9 @@
         </is>
       </c>
       <c r="J407" t="n">
+        <v>6</v>
+      </c>
+      <c r="K407" t="n">
         <v>1</v>
       </c>
       <c r="L407" t="inlineStr">
@@ -28505,6 +29723,9 @@
         </is>
       </c>
       <c r="J408" t="n">
+        <v>6</v>
+      </c>
+      <c r="K408" t="n">
         <v>1</v>
       </c>
       <c r="L408" t="inlineStr">
@@ -28574,6 +29795,9 @@
         </is>
       </c>
       <c r="J409" t="n">
+        <v>6</v>
+      </c>
+      <c r="K409" t="n">
         <v>1</v>
       </c>
       <c r="L409" t="inlineStr">
@@ -28643,6 +29867,9 @@
         </is>
       </c>
       <c r="J410" t="n">
+        <v>6</v>
+      </c>
+      <c r="K410" t="n">
         <v>1</v>
       </c>
       <c r="L410" t="inlineStr">
@@ -28714,6 +29941,9 @@
       <c r="J411" t="n">
         <v>1</v>
       </c>
+      <c r="K411" t="n">
+        <v>1</v>
+      </c>
       <c r="L411" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -28783,6 +30013,9 @@
       <c r="J412" t="n">
         <v>1</v>
       </c>
+      <c r="K412" t="n">
+        <v>1</v>
+      </c>
       <c r="L412" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -28852,6 +30085,9 @@
       <c r="J413" t="n">
         <v>1</v>
       </c>
+      <c r="K413" t="n">
+        <v>1</v>
+      </c>
       <c r="L413" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -28921,6 +30157,9 @@
       <c r="J414" t="n">
         <v>1</v>
       </c>
+      <c r="K414" t="n">
+        <v>1</v>
+      </c>
       <c r="L414" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -28990,6 +30229,9 @@
       <c r="J415" t="n">
         <v>1</v>
       </c>
+      <c r="K415" t="n">
+        <v>1</v>
+      </c>
       <c r="L415" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -29057,6 +30299,9 @@
         </is>
       </c>
       <c r="J416" t="n">
+        <v>1</v>
+      </c>
+      <c r="K416" t="n">
         <v>2</v>
       </c>
       <c r="L416" t="inlineStr">
@@ -29126,6 +30371,9 @@
         </is>
       </c>
       <c r="J417" t="n">
+        <v>1</v>
+      </c>
+      <c r="K417" t="n">
         <v>2</v>
       </c>
       <c r="L417" t="inlineStr">
@@ -29195,6 +30443,9 @@
         </is>
       </c>
       <c r="J418" t="n">
+        <v>1</v>
+      </c>
+      <c r="K418" t="n">
         <v>2</v>
       </c>
       <c r="L418" t="inlineStr">
@@ -29264,6 +30515,9 @@
         </is>
       </c>
       <c r="J419" t="n">
+        <v>1</v>
+      </c>
+      <c r="K419" t="n">
         <v>2</v>
       </c>
       <c r="L419" t="inlineStr">
@@ -29333,6 +30587,9 @@
         </is>
       </c>
       <c r="J420" t="n">
+        <v>1</v>
+      </c>
+      <c r="K420" t="n">
         <v>2</v>
       </c>
       <c r="L420" t="inlineStr">
@@ -29402,6 +30659,9 @@
         </is>
       </c>
       <c r="J421" t="n">
+        <v>1</v>
+      </c>
+      <c r="K421" t="n">
         <v>2</v>
       </c>
       <c r="L421" t="inlineStr">
@@ -29471,6 +30731,9 @@
         </is>
       </c>
       <c r="J422" t="n">
+        <v>1</v>
+      </c>
+      <c r="K422" t="n">
         <v>2</v>
       </c>
       <c r="L422" t="inlineStr">
@@ -29540,6 +30803,9 @@
         </is>
       </c>
       <c r="J423" t="n">
+        <v>1</v>
+      </c>
+      <c r="K423" t="n">
         <v>2</v>
       </c>
       <c r="L423" t="inlineStr">
@@ -29609,6 +30875,9 @@
         </is>
       </c>
       <c r="J424" t="n">
+        <v>1</v>
+      </c>
+      <c r="K424" t="n">
         <v>2</v>
       </c>
       <c r="L424" t="inlineStr">
@@ -29678,6 +30947,9 @@
         </is>
       </c>
       <c r="J425" t="n">
+        <v>1</v>
+      </c>
+      <c r="K425" t="n">
         <v>2</v>
       </c>
       <c r="L425" t="inlineStr">
@@ -29747,6 +31019,9 @@
         </is>
       </c>
       <c r="J426" t="n">
+        <v>1</v>
+      </c>
+      <c r="K426" t="n">
         <v>2</v>
       </c>
       <c r="L426" t="inlineStr">
@@ -29816,6 +31091,9 @@
         </is>
       </c>
       <c r="J427" t="n">
+        <v>1</v>
+      </c>
+      <c r="K427" t="n">
         <v>2</v>
       </c>
       <c r="L427" t="inlineStr">
@@ -29885,6 +31163,9 @@
         </is>
       </c>
       <c r="J428" t="n">
+        <v>1</v>
+      </c>
+      <c r="K428" t="n">
         <v>2</v>
       </c>
       <c r="L428" t="inlineStr">
@@ -29954,6 +31235,9 @@
         </is>
       </c>
       <c r="J429" t="n">
+        <v>1</v>
+      </c>
+      <c r="K429" t="n">
         <v>2</v>
       </c>
       <c r="L429" t="inlineStr">
@@ -30023,6 +31307,9 @@
         </is>
       </c>
       <c r="J430" t="n">
+        <v>1</v>
+      </c>
+      <c r="K430" t="n">
         <v>2</v>
       </c>
       <c r="L430" t="inlineStr">
@@ -30092,6 +31379,9 @@
         </is>
       </c>
       <c r="J431" t="n">
+        <v>1</v>
+      </c>
+      <c r="K431" t="n">
         <v>2</v>
       </c>
       <c r="L431" t="inlineStr">
@@ -30161,6 +31451,9 @@
         </is>
       </c>
       <c r="J432" t="n">
+        <v>1</v>
+      </c>
+      <c r="K432" t="n">
         <v>2</v>
       </c>
       <c r="L432" t="inlineStr">
@@ -30230,6 +31523,9 @@
         </is>
       </c>
       <c r="J433" t="n">
+        <v>1</v>
+      </c>
+      <c r="K433" t="n">
         <v>2</v>
       </c>
       <c r="L433" t="inlineStr">
@@ -30301,6 +31597,9 @@
       <c r="J434" t="n">
         <v>1</v>
       </c>
+      <c r="K434" t="n">
+        <v>1</v>
+      </c>
       <c r="L434" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -30370,6 +31669,9 @@
       <c r="J435" t="n">
         <v>1</v>
       </c>
+      <c r="K435" t="n">
+        <v>1</v>
+      </c>
       <c r="L435" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -30439,6 +31741,9 @@
       <c r="J436" t="n">
         <v>1</v>
       </c>
+      <c r="K436" t="n">
+        <v>1</v>
+      </c>
       <c r="L436" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -30506,6 +31811,9 @@
         </is>
       </c>
       <c r="J437" t="n">
+        <v>1</v>
+      </c>
+      <c r="K437" t="n">
         <v>2</v>
       </c>
       <c r="L437" t="inlineStr">
@@ -30575,6 +31883,9 @@
         </is>
       </c>
       <c r="J438" t="n">
+        <v>1</v>
+      </c>
+      <c r="K438" t="n">
         <v>2</v>
       </c>
       <c r="L438" t="inlineStr">
@@ -30644,6 +31955,9 @@
         </is>
       </c>
       <c r="J439" t="n">
+        <v>1</v>
+      </c>
+      <c r="K439" t="n">
         <v>2</v>
       </c>
       <c r="L439" t="inlineStr">
@@ -30715,6 +32029,9 @@
       <c r="J440" t="n">
         <v>1</v>
       </c>
+      <c r="K440" t="n">
+        <v>1</v>
+      </c>
       <c r="L440" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -30784,6 +32101,9 @@
       <c r="J441" t="n">
         <v>1</v>
       </c>
+      <c r="K441" t="n">
+        <v>1</v>
+      </c>
       <c r="L441" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -30853,6 +32173,9 @@
       <c r="J442" t="n">
         <v>1</v>
       </c>
+      <c r="K442" t="n">
+        <v>1</v>
+      </c>
       <c r="L442" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -30922,6 +32245,9 @@
       <c r="J443" t="n">
         <v>1</v>
       </c>
+      <c r="K443" t="n">
+        <v>1</v>
+      </c>
       <c r="L443" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -30991,6 +32317,9 @@
       <c r="J444" t="n">
         <v>1</v>
       </c>
+      <c r="K444" t="n">
+        <v>1</v>
+      </c>
       <c r="L444" t="inlineStr">
         <is>
           <t>Obligatoria</t>
@@ -31058,6 +32387,9 @@
         </is>
       </c>
       <c r="J445" t="n">
+        <v>1</v>
+      </c>
+      <c r="K445" t="n">
         <v>2</v>
       </c>
       <c r="L445" t="inlineStr">
@@ -31127,6 +32459,9 @@
         </is>
       </c>
       <c r="J446" t="n">
+        <v>1</v>
+      </c>
+      <c r="K446" t="n">
         <v>2</v>
       </c>
       <c r="L446" t="inlineStr">
@@ -31196,6 +32531,9 @@
         </is>
       </c>
       <c r="J447" t="n">
+        <v>1</v>
+      </c>
+      <c r="K447" t="n">
         <v>2</v>
       </c>
       <c r="L447" t="inlineStr">
@@ -31267,6 +32605,9 @@
       <c r="J448" t="n">
         <v>1</v>
       </c>
+      <c r="K448" t="n">
+        <v>1</v>
+      </c>
       <c r="L448" t="inlineStr">
         <is>
           <t>Opcional</t>
@@ -31336,6 +32677,9 @@
       <c r="J449" t="n">
         <v>1</v>
       </c>
+      <c r="K449" t="n">
+        <v>1</v>
+      </c>
       <c r="L449" t="inlineStr">
         <is>
           <t>Opcional</t>
@@ -31405,6 +32749,9 @@
       <c r="J450" t="n">
         <v>1</v>
       </c>
+      <c r="K450" t="n">
+        <v>1</v>
+      </c>
       <c r="L450" t="inlineStr">
         <is>
           <t>Opcional</t>
@@ -31472,6 +32819,9 @@
         </is>
       </c>
       <c r="J451" t="n">
+        <v>1</v>
+      </c>
+      <c r="K451" t="n">
         <v>2</v>
       </c>
       <c r="L451" t="inlineStr">
@@ -31541,6 +32891,9 @@
         </is>
       </c>
       <c r="J452" t="n">
+        <v>1</v>
+      </c>
+      <c r="K452" t="n">
         <v>2</v>
       </c>
       <c r="L452" t="inlineStr">
@@ -31610,6 +32963,9 @@
         </is>
       </c>
       <c r="J453" t="n">
+        <v>1</v>
+      </c>
+      <c r="K453" t="n">
         <v>2</v>
       </c>
       <c r="L453" t="inlineStr">
@@ -31679,6 +33035,9 @@
         </is>
       </c>
       <c r="J454" t="n">
+        <v>1</v>
+      </c>
+      <c r="K454" t="n">
         <v>2</v>
       </c>
       <c r="L454" t="inlineStr">
@@ -31748,6 +33107,9 @@
         </is>
       </c>
       <c r="J455" t="n">
+        <v>1</v>
+      </c>
+      <c r="K455" t="n">
         <v>2</v>
       </c>
       <c r="L455" t="inlineStr">
@@ -31817,6 +33179,9 @@
         </is>
       </c>
       <c r="J456" t="n">
+        <v>1</v>
+      </c>
+      <c r="K456" t="n">
         <v>2</v>
       </c>
       <c r="L456" t="inlineStr">
@@ -31886,6 +33251,9 @@
         </is>
       </c>
       <c r="J457" t="n">
+        <v>2</v>
+      </c>
+      <c r="K457" t="n">
         <v>1</v>
       </c>
       <c r="L457" t="inlineStr">
@@ -31955,6 +33323,9 @@
         </is>
       </c>
       <c r="J458" t="n">
+        <v>2</v>
+      </c>
+      <c r="K458" t="n">
         <v>1</v>
       </c>
       <c r="L458" t="inlineStr">
@@ -32026,6 +33397,9 @@
       <c r="J459" t="n">
         <v>3</v>
       </c>
+      <c r="K459" t="n">
+        <v>3</v>
+      </c>
       <c r="L459" t="inlineStr">
         <is>
           <t>Opcional</t>
@@ -32095,6 +33469,9 @@
       <c r="J460" t="n">
         <v>3</v>
       </c>
+      <c r="K460" t="n">
+        <v>3</v>
+      </c>
       <c r="L460" t="inlineStr">
         <is>
           <t>Opcional</t>
@@ -32162,6 +33539,9 @@
         </is>
       </c>
       <c r="J461" t="n">
+        <v>3</v>
+      </c>
+      <c r="K461" t="n">
         <v>0</v>
       </c>
       <c r="L461" t="inlineStr">
@@ -32231,6 +33611,9 @@
         </is>
       </c>
       <c r="J462" t="n">
+        <v>1</v>
+      </c>
+      <c r="K462" t="n">
         <v>0</v>
       </c>
       <c r="L462" t="inlineStr">
@@ -32300,6 +33683,9 @@
         </is>
       </c>
       <c r="J463" t="n">
+        <v>2</v>
+      </c>
+      <c r="K463" t="n">
         <v>0</v>
       </c>
       <c r="L463" t="inlineStr">
@@ -32369,6 +33755,9 @@
         </is>
       </c>
       <c r="J464" t="n">
+        <v>3</v>
+      </c>
+      <c r="K464" t="n">
         <v>0</v>
       </c>
       <c r="L464" t="inlineStr">

</xml_diff>